<commit_message>
Practica 5 finalizada y revisada
</commit_message>
<xml_diff>
--- a/resources/SistemasAgua.xlsx
+++ b/resources/SistemasAgua.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="611">
   <si>
     <t>Nombre</t>
   </si>
@@ -1557,7 +1557,319 @@
     <t>S</t>
   </si>
   <si>
+    <t>DK7331645124473461205164</t>
+  </si>
+  <si>
+    <t>ES8265614874165615445616</t>
+  </si>
+  <si>
+    <t>RO8832569523016220165156</t>
+  </si>
+  <si>
+    <t>DE7424561937521546497521</t>
+  </si>
+  <si>
+    <t>MC6436520125638451012515</t>
+  </si>
+  <si>
+    <t>ES0721584976902154655487</t>
+  </si>
+  <si>
+    <t>GR9420125003305201112544</t>
+  </si>
+  <si>
+    <t>ES2821651484690980008984</t>
+  </si>
+  <si>
+    <t>FI5620960043043554600000</t>
+  </si>
+  <si>
+    <t>ES7921564975243245467995</t>
+  </si>
+  <si>
+    <t>LT8032566221522587754554</t>
+  </si>
+  <si>
+    <t>EE2023215465315456411515</t>
+  </si>
+  <si>
+    <t>BE9400750184310702510000</t>
+  </si>
+  <si>
+    <t>SM2125894363475485700145</t>
+  </si>
+  <si>
+    <t>ES9596431245118150005156</t>
+  </si>
+  <si>
     <t>09548416N</t>
+  </si>
+  <si>
+    <t>AT6825030000114574745458</t>
+  </si>
+  <si>
+    <t>IT8915953684811254695203</t>
+  </si>
+  <si>
+    <t>ES9020960043023096200000</t>
+  </si>
+  <si>
+    <t>DK5800750184310702510000</t>
+  </si>
+  <si>
+    <t>ES5023455254943263234457</t>
+  </si>
+  <si>
+    <t>GR4920910936583000000000</t>
+  </si>
+  <si>
+    <t>ES3720960043032159000000</t>
+  </si>
+  <si>
+    <t>DE5512669681115112121210</t>
+  </si>
+  <si>
+    <t>ES2956187775315550000651</t>
+  </si>
+  <si>
+    <t>ES0425516848021156151054</t>
+  </si>
+  <si>
+    <t>PT5764578946740051516490</t>
+  </si>
+  <si>
+    <t>ES4534698752714600549403</t>
+  </si>
+  <si>
+    <t>ES2766649444162310000255</t>
+  </si>
+  <si>
+    <t>FR5623185484465641685100</t>
+  </si>
+  <si>
+    <t>DE5021508149175421346497</t>
+  </si>
+  <si>
+    <t>DE6721346154503164978451</t>
+  </si>
+  <si>
+    <t>ES7225187786311225455548</t>
+  </si>
+  <si>
+    <t>ES4723164897642213030615</t>
+  </si>
+  <si>
+    <t>ES2396536214865214585214</t>
+  </si>
+  <si>
+    <t>ES6885461325251978750005</t>
+  </si>
+  <si>
+    <t>FI5024587946032003165464</t>
+  </si>
+  <si>
+    <t>ES5020960043073071400000</t>
+  </si>
+  <si>
+    <t>ES8220960043042158800000</t>
+  </si>
+  <si>
+    <t>ES7521654587985156484454</t>
+  </si>
+  <si>
+    <t>ES3251651681961210656510</t>
+  </si>
+  <si>
+    <t>ES5566552211148855332200</t>
+  </si>
+  <si>
+    <t>GB9720910936583000000000</t>
+  </si>
+  <si>
+    <t>DE9301821135910205540000</t>
+  </si>
+  <si>
+    <t>DE7822631245526916432102</t>
+  </si>
+  <si>
+    <t>ES2120960043043075700000</t>
+  </si>
+  <si>
+    <t>SM7325635478321002541225</t>
+  </si>
+  <si>
+    <t>ES6832154697195423121000</t>
+  </si>
+  <si>
+    <t>GR3836521452736500658485</t>
+  </si>
+  <si>
+    <t>GB5520008521528775113366</t>
+  </si>
+  <si>
+    <t>ES8020960043033000100000</t>
+  </si>
+  <si>
+    <t>GB0836585214290025478551</t>
+  </si>
+  <si>
+    <t>ES9012548523465214585214</t>
+  </si>
+  <si>
+    <t>ES6931624561042546920007</t>
+  </si>
+  <si>
+    <t>ES1436154231712500312566</t>
+  </si>
+  <si>
+    <t>ES8244875664127231645789</t>
+  </si>
+  <si>
+    <t>ES7920960031442124800000</t>
+  </si>
+  <si>
+    <t>ES1633620012937852100256</t>
+  </si>
+  <si>
+    <t>ES1933218885441445121022</t>
+  </si>
+  <si>
+    <t>ES8462581542713690044508</t>
+  </si>
+  <si>
+    <t>ES3925165151118666365100</t>
+  </si>
+  <si>
+    <t>PT3536952365020014425254</t>
+  </si>
+  <si>
+    <t>ES9565168874641561561500</t>
+  </si>
+  <si>
+    <t>ES3220960583831234500000</t>
+  </si>
+  <si>
+    <t>ES7221416325811510005514</t>
+  </si>
+  <si>
+    <t>LU0932628484504115151115</t>
+  </si>
+  <si>
+    <t>20960056133231500000</t>
+  </si>
+  <si>
+    <t>ES2220960056133231500000</t>
+  </si>
+  <si>
+    <t>ES8163516541828944000984</t>
+  </si>
+  <si>
+    <t>23658965274585223202</t>
+  </si>
+  <si>
+    <t>ES6223658965274585223202</t>
+  </si>
+  <si>
+    <t>FI6132658012367712548745</t>
+  </si>
+  <si>
+    <t>ES7223652365142254222000</t>
+  </si>
+  <si>
+    <t>20012541150023365233</t>
+  </si>
+  <si>
+    <t>FR3820012541150023365233</t>
+  </si>
+  <si>
+    <t>ES9232584216971684051000</t>
+  </si>
+  <si>
+    <t>ES7395485212315484010000</t>
+  </si>
+  <si>
+    <t>LT9321856333126985542360</t>
+  </si>
+  <si>
+    <t>ES5736245978133245679001</t>
+  </si>
+  <si>
+    <t>ES7631245164156597845124</t>
+  </si>
+  <si>
+    <t>SM4423221158252545471411</t>
+  </si>
+  <si>
+    <t>SE6832574512085411002255</t>
+  </si>
+  <si>
+    <t>ES4420960043013468900000</t>
+  </si>
+  <si>
+    <t>ES5631215643855060225021</t>
+  </si>
+  <si>
+    <t>AT3285550564726165145610</t>
+  </si>
+  <si>
+    <t>ES1665165654918886005001</t>
+  </si>
+  <si>
+    <t>65645150865168448896</t>
+  </si>
+  <si>
+    <t>AT8365645150865168448896</t>
+  </si>
+  <si>
+    <t>26551681807651415636</t>
+  </si>
+  <si>
+    <t>IT3526551681807651415636</t>
+  </si>
+  <si>
+    <t>HU2399558741836555551120</t>
+  </si>
+  <si>
+    <t>ES4352198484752100515144</t>
+  </si>
+  <si>
+    <t>51556584221251000254</t>
+  </si>
+  <si>
+    <t>IE6851556584221251000254</t>
+  </si>
+  <si>
+    <t>DK9032541112811220000588</t>
+  </si>
+  <si>
+    <t>62541122421110105611</t>
+  </si>
+  <si>
+    <t>LT9362541122421110105611</t>
+  </si>
+  <si>
+    <t>ES6855065688761051056105</t>
+  </si>
+  <si>
+    <t>ES7426221011628048788896</t>
+  </si>
+  <si>
+    <t>ES9712548521518742146695</t>
+  </si>
+  <si>
+    <t>ES9001826530120201560000</t>
+  </si>
+  <si>
+    <t>ES9021651651812511133551</t>
+  </si>
+  <si>
+    <t>ES6851651487910005118185</t>
+  </si>
+  <si>
+    <t>CZ9536250012804785523365</t>
+  </si>
+  <si>
+    <t>AT3122515651915640081000</t>
   </si>
 </sst>
 </file>
@@ -2027,6 +2339,9 @@
       <c r="H2" s="3" t="s">
         <v>267</v>
       </c>
+      <c r="I2" t="s" s="0">
+        <v>506</v>
+      </c>
       <c r="K2" t="s" s="0">
         <v>264</v>
       </c>
@@ -2071,6 +2386,9 @@
       <c r="H3" s="3" t="s">
         <v>268</v>
       </c>
+      <c r="I3" t="s" s="0">
+        <v>507</v>
+      </c>
       <c r="K3" t="s" s="0">
         <v>264</v>
       </c>
@@ -2115,6 +2433,9 @@
       <c r="H4" s="3" t="s">
         <v>269</v>
       </c>
+      <c r="I4" t="s" s="0">
+        <v>508</v>
+      </c>
       <c r="K4" t="s" s="0">
         <v>264</v>
       </c>
@@ -2159,6 +2480,9 @@
       <c r="H5" s="3" t="s">
         <v>270</v>
       </c>
+      <c r="I5" t="s" s="0">
+        <v>509</v>
+      </c>
       <c r="K5" t="s" s="0">
         <v>264</v>
       </c>
@@ -2203,6 +2527,9 @@
       <c r="H6" s="3" t="s">
         <v>271</v>
       </c>
+      <c r="I6" t="s" s="0">
+        <v>510</v>
+      </c>
       <c r="K6" t="s" s="0">
         <v>264</v>
       </c>
@@ -2247,6 +2574,9 @@
       <c r="H7" s="3" t="s">
         <v>272</v>
       </c>
+      <c r="I7" t="s" s="0">
+        <v>511</v>
+      </c>
       <c r="K7" t="s" s="0">
         <v>264</v>
       </c>
@@ -2291,6 +2621,9 @@
       <c r="H8" s="3" t="s">
         <v>273</v>
       </c>
+      <c r="I8" t="s" s="0">
+        <v>512</v>
+      </c>
       <c r="K8" t="s" s="0">
         <v>264</v>
       </c>
@@ -2335,6 +2668,9 @@
       <c r="H9" s="3" t="s">
         <v>274</v>
       </c>
+      <c r="I9" t="s" s="0">
+        <v>513</v>
+      </c>
       <c r="K9" t="s" s="0">
         <v>264</v>
       </c>
@@ -2379,6 +2715,9 @@
       <c r="H10" s="3" t="s">
         <v>275</v>
       </c>
+      <c r="I10" t="s" s="0">
+        <v>514</v>
+      </c>
       <c r="K10" t="s" s="0">
         <v>264</v>
       </c>
@@ -2423,6 +2762,9 @@
       <c r="H11" s="3" t="s">
         <v>276</v>
       </c>
+      <c r="I11" t="s" s="0">
+        <v>515</v>
+      </c>
       <c r="K11" t="s" s="0">
         <v>264</v>
       </c>
@@ -2467,6 +2809,9 @@
       <c r="H12" s="3" t="s">
         <v>277</v>
       </c>
+      <c r="I12" t="s" s="0">
+        <v>516</v>
+      </c>
       <c r="K12" t="s" s="0">
         <v>264</v>
       </c>
@@ -2511,6 +2856,9 @@
       <c r="H13" s="3" t="s">
         <v>278</v>
       </c>
+      <c r="I13" t="s" s="0">
+        <v>517</v>
+      </c>
       <c r="K13" t="s" s="0">
         <v>264</v>
       </c>
@@ -2554,6 +2902,9 @@
       </c>
       <c r="H14" s="3" t="s">
         <v>279</v>
+      </c>
+      <c r="I14" t="s" s="0">
+        <v>518</v>
       </c>
       <c r="K14" t="s" s="0">
         <v>264</v>
@@ -2605,6 +2956,9 @@
       <c r="H16" s="3" t="s">
         <v>280</v>
       </c>
+      <c r="I16" t="s" s="0">
+        <v>519</v>
+      </c>
       <c r="K16" t="s" s="0">
         <v>264</v>
       </c>
@@ -2649,6 +3003,9 @@
       <c r="H17" s="3" t="s">
         <v>281</v>
       </c>
+      <c r="I17" t="s" s="0">
+        <v>520</v>
+      </c>
       <c r="K17" t="s" s="0">
         <v>264</v>
       </c>
@@ -2679,7 +3036,7 @@
         <v>144</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>506</v>
+        <v>521</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>393</v>
@@ -2692,6 +3049,9 @@
       </c>
       <c r="H18" s="3" t="s">
         <v>282</v>
+      </c>
+      <c r="I18" t="s" s="0">
+        <v>522</v>
       </c>
       <c r="K18" t="s" s="0">
         <v>264</v>
@@ -2737,6 +3097,9 @@
       <c r="H19" s="3" t="s">
         <v>283</v>
       </c>
+      <c r="I19" t="s" s="0">
+        <v>523</v>
+      </c>
       <c r="K19" t="s" s="0">
         <v>264</v>
       </c>
@@ -2781,6 +3144,9 @@
       <c r="H20" s="3" t="s">
         <v>284</v>
       </c>
+      <c r="I20" t="s" s="0">
+        <v>524</v>
+      </c>
       <c r="K20" t="s" s="0">
         <v>264</v>
       </c>
@@ -2825,6 +3191,9 @@
       <c r="H21" s="3" t="s">
         <v>279</v>
       </c>
+      <c r="I21" t="s" s="0">
+        <v>525</v>
+      </c>
       <c r="K21" t="s" s="0">
         <v>264</v>
       </c>
@@ -2866,6 +3235,9 @@
       <c r="H22" s="3" t="s">
         <v>285</v>
       </c>
+      <c r="I22" t="s" s="0">
+        <v>526</v>
+      </c>
       <c r="K22" t="s" s="0">
         <v>264</v>
       </c>
@@ -2907,6 +3279,9 @@
       <c r="H23" s="3" t="s">
         <v>286</v>
       </c>
+      <c r="I23" t="s" s="0">
+        <v>527</v>
+      </c>
       <c r="K23" t="s" s="0">
         <v>264</v>
       </c>
@@ -2948,6 +3323,9 @@
       <c r="H24" s="3" t="s">
         <v>287</v>
       </c>
+      <c r="I24" t="s" s="0">
+        <v>528</v>
+      </c>
       <c r="K24" t="s" s="0">
         <v>264</v>
       </c>
@@ -2988,6 +3366,9 @@
       </c>
       <c r="H25" s="3" t="s">
         <v>288</v>
+      </c>
+      <c r="I25" t="s" s="0">
+        <v>529</v>
       </c>
       <c r="K25" t="s" s="0">
         <v>264</v>
@@ -3039,6 +3420,9 @@
       <c r="H27" s="3" t="s">
         <v>289</v>
       </c>
+      <c r="I27" t="s" s="0">
+        <v>530</v>
+      </c>
       <c r="K27" t="s" s="0">
         <v>264</v>
       </c>
@@ -3083,6 +3467,9 @@
       <c r="H28" s="3" t="s">
         <v>290</v>
       </c>
+      <c r="I28" t="s" s="0">
+        <v>531</v>
+      </c>
       <c r="K28" t="s" s="0">
         <v>264</v>
       </c>
@@ -3127,6 +3514,9 @@
       <c r="H29" s="3" t="s">
         <v>291</v>
       </c>
+      <c r="I29" t="s" s="0">
+        <v>532</v>
+      </c>
       <c r="K29" t="s" s="0">
         <v>264</v>
       </c>
@@ -3171,6 +3561,9 @@
       <c r="H30" s="3" t="s">
         <v>292</v>
       </c>
+      <c r="I30" t="s" s="0">
+        <v>533</v>
+      </c>
       <c r="K30" t="s" s="0">
         <v>264</v>
       </c>
@@ -3215,6 +3608,9 @@
       <c r="H31" s="3" t="s">
         <v>293</v>
       </c>
+      <c r="I31" t="s" s="0">
+        <v>534</v>
+      </c>
       <c r="K31" t="s" s="0">
         <v>264</v>
       </c>
@@ -3258,6 +3654,9 @@
       </c>
       <c r="H32" s="3" t="s">
         <v>294</v>
+      </c>
+      <c r="I32" t="s" s="0">
+        <v>535</v>
       </c>
       <c r="K32" t="s" s="0">
         <v>264</v>
@@ -3321,6 +3720,9 @@
       <c r="H36" s="3" t="s">
         <v>295</v>
       </c>
+      <c r="I36" t="s" s="0">
+        <v>536</v>
+      </c>
       <c r="K36" t="s" s="0">
         <v>264</v>
       </c>
@@ -3365,6 +3767,9 @@
       <c r="H37" s="3" t="s">
         <v>296</v>
       </c>
+      <c r="I37" t="s" s="0">
+        <v>537</v>
+      </c>
       <c r="K37" t="s" s="0">
         <v>264</v>
       </c>
@@ -3409,6 +3814,9 @@
       <c r="H38" s="3" t="s">
         <v>297</v>
       </c>
+      <c r="I38" t="s" s="0">
+        <v>538</v>
+      </c>
       <c r="K38" t="s" s="0">
         <v>264</v>
       </c>
@@ -3453,6 +3861,9 @@
       <c r="H39" s="3" t="s">
         <v>298</v>
       </c>
+      <c r="I39" t="s" s="0">
+        <v>539</v>
+      </c>
       <c r="K39" t="s" s="0">
         <v>264</v>
       </c>
@@ -3497,6 +3908,9 @@
       <c r="H40" s="3" t="s">
         <v>299</v>
       </c>
+      <c r="I40" t="s" s="0">
+        <v>540</v>
+      </c>
       <c r="K40" t="s" s="0">
         <v>264</v>
       </c>
@@ -3541,6 +3955,9 @@
       <c r="H41" s="3" t="s">
         <v>300</v>
       </c>
+      <c r="I41" t="s" s="0">
+        <v>541</v>
+      </c>
       <c r="K41" t="s" s="0">
         <v>264</v>
       </c>
@@ -3585,6 +4002,9 @@
       <c r="H42" s="3" t="s">
         <v>301</v>
       </c>
+      <c r="I42" t="s" s="0">
+        <v>542</v>
+      </c>
       <c r="K42" t="s" s="0">
         <v>264</v>
       </c>
@@ -3629,6 +4049,9 @@
       <c r="H43" s="3" t="s">
         <v>302</v>
       </c>
+      <c r="I43" t="s" s="0">
+        <v>543</v>
+      </c>
       <c r="K43" t="s" s="0">
         <v>264</v>
       </c>
@@ -3673,6 +4096,9 @@
       <c r="H44" s="3" t="s">
         <v>303</v>
       </c>
+      <c r="I44" t="s" s="0">
+        <v>544</v>
+      </c>
       <c r="K44" t="s" s="0">
         <v>264</v>
       </c>
@@ -3717,6 +4143,9 @@
       <c r="H45" s="3" t="s">
         <v>304</v>
       </c>
+      <c r="I45" t="s" s="0">
+        <v>545</v>
+      </c>
       <c r="K45" t="s" s="0">
         <v>264</v>
       </c>
@@ -3761,6 +4190,9 @@
       <c r="H46" s="3" t="s">
         <v>305</v>
       </c>
+      <c r="I46" t="s" s="0">
+        <v>546</v>
+      </c>
       <c r="K46" t="s" s="0">
         <v>264</v>
       </c>
@@ -3805,6 +4237,9 @@
       <c r="H47" s="3" t="s">
         <v>306</v>
       </c>
+      <c r="I47" t="s" s="0">
+        <v>547</v>
+      </c>
       <c r="K47" t="s" s="0">
         <v>264</v>
       </c>
@@ -3849,6 +4284,9 @@
       <c r="H48" s="3" t="s">
         <v>286</v>
       </c>
+      <c r="I48" t="s" s="0">
+        <v>548</v>
+      </c>
       <c r="K48" t="s" s="0">
         <v>264</v>
       </c>
@@ -3893,6 +4331,9 @@
       <c r="H49" s="3" t="s">
         <v>307</v>
       </c>
+      <c r="I49" t="s" s="0">
+        <v>549</v>
+      </c>
       <c r="K49" t="s" s="0">
         <v>264</v>
       </c>
@@ -3937,6 +4378,9 @@
       <c r="H50" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="I50" t="s" s="0">
+        <v>550</v>
+      </c>
       <c r="K50" t="s" s="0">
         <v>264</v>
       </c>
@@ -3981,6 +4425,9 @@
       <c r="H51" s="3" t="s">
         <v>309</v>
       </c>
+      <c r="I51" t="s" s="0">
+        <v>551</v>
+      </c>
       <c r="K51" t="s" s="0">
         <v>264</v>
       </c>
@@ -4025,6 +4472,9 @@
       <c r="H52" s="3" t="s">
         <v>310</v>
       </c>
+      <c r="I52" t="s" s="0">
+        <v>552</v>
+      </c>
       <c r="K52" t="s" s="0">
         <v>264</v>
       </c>
@@ -4069,6 +4519,9 @@
       <c r="H53" s="3" t="s">
         <v>311</v>
       </c>
+      <c r="I53" t="s" s="0">
+        <v>553</v>
+      </c>
       <c r="K53" t="s" s="0">
         <v>264</v>
       </c>
@@ -4113,6 +4566,9 @@
       <c r="H54" s="3" t="s">
         <v>312</v>
       </c>
+      <c r="I54" t="s" s="0">
+        <v>554</v>
+      </c>
       <c r="K54" t="s" s="0">
         <v>264</v>
       </c>
@@ -4156,6 +4612,9 @@
       </c>
       <c r="H55" s="3" t="s">
         <v>313</v>
+      </c>
+      <c r="I55" t="s" s="0">
+        <v>555</v>
       </c>
       <c r="K55" t="s" s="0">
         <v>264</v>
@@ -4225,6 +4684,9 @@
       <c r="H60" s="3" t="s">
         <v>314</v>
       </c>
+      <c r="I60" t="s" s="0">
+        <v>556</v>
+      </c>
       <c r="K60" t="s" s="0">
         <v>264</v>
       </c>
@@ -4269,6 +4731,9 @@
       <c r="H61" s="3" t="s">
         <v>315</v>
       </c>
+      <c r="I61" t="s" s="0">
+        <v>557</v>
+      </c>
       <c r="K61" t="s" s="0">
         <v>264</v>
       </c>
@@ -4313,6 +4778,9 @@
       <c r="H62" s="3" t="s">
         <v>316</v>
       </c>
+      <c r="I62" t="s" s="0">
+        <v>558</v>
+      </c>
       <c r="K62" t="s" s="0">
         <v>264</v>
       </c>
@@ -4357,6 +4825,9 @@
       <c r="H63" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="I63" t="s" s="0">
+        <v>559</v>
+      </c>
       <c r="K63" t="s" s="0">
         <v>264</v>
       </c>
@@ -4398,6 +4869,9 @@
       <c r="H64" s="3" t="s">
         <v>318</v>
       </c>
+      <c r="I64" t="s" s="0">
+        <v>560</v>
+      </c>
       <c r="K64" t="s" s="0">
         <v>264</v>
       </c>
@@ -4439,6 +4913,9 @@
       <c r="H65" s="3" t="s">
         <v>319</v>
       </c>
+      <c r="I65" t="s" s="0">
+        <v>561</v>
+      </c>
       <c r="K65" t="s" s="0">
         <v>264</v>
       </c>
@@ -4480,6 +4957,9 @@
       <c r="H66" s="3" t="s">
         <v>320</v>
       </c>
+      <c r="I66" t="s" s="0">
+        <v>562</v>
+      </c>
       <c r="K66" t="s" s="0">
         <v>264</v>
       </c>
@@ -4524,6 +5004,9 @@
       <c r="H67" s="3" t="s">
         <v>321</v>
       </c>
+      <c r="I67" t="s" s="0">
+        <v>563</v>
+      </c>
       <c r="K67" t="s" s="0">
         <v>264</v>
       </c>
@@ -4568,6 +5051,9 @@
       <c r="H68" s="3" t="s">
         <v>322</v>
       </c>
+      <c r="I68" t="s" s="0">
+        <v>564</v>
+      </c>
       <c r="K68" t="s" s="0">
         <v>264</v>
       </c>
@@ -4612,6 +5098,9 @@
       <c r="H69" s="3" t="s">
         <v>323</v>
       </c>
+      <c r="I69" t="s" s="0">
+        <v>565</v>
+      </c>
       <c r="K69" t="s" s="0">
         <v>264</v>
       </c>
@@ -4656,6 +5145,9 @@
       <c r="H70" s="3" t="s">
         <v>324</v>
       </c>
+      <c r="I70" t="s" s="0">
+        <v>566</v>
+      </c>
       <c r="K70" t="s" s="0">
         <v>264</v>
       </c>
@@ -4700,6 +5192,9 @@
       <c r="H71" s="3" t="s">
         <v>314</v>
       </c>
+      <c r="I71" t="s" s="0">
+        <v>556</v>
+      </c>
       <c r="K71" t="s" s="0">
         <v>264</v>
       </c>
@@ -4744,6 +5239,9 @@
       <c r="H72" s="3" t="s">
         <v>325</v>
       </c>
+      <c r="I72" t="s" s="0">
+        <v>567</v>
+      </c>
       <c r="K72" t="s" s="0">
         <v>264</v>
       </c>
@@ -4788,6 +5286,9 @@
       <c r="H73" s="3" t="s">
         <v>326</v>
       </c>
+      <c r="I73" t="s" s="0">
+        <v>568</v>
+      </c>
       <c r="K73" t="s" s="0">
         <v>264</v>
       </c>
@@ -4832,6 +5333,9 @@
       <c r="H74" s="3" t="s">
         <v>327</v>
       </c>
+      <c r="I74" t="s" s="0">
+        <v>569</v>
+      </c>
       <c r="K74" t="s" s="0">
         <v>264</v>
       </c>
@@ -4876,6 +5380,9 @@
       <c r="H75" s="3" t="s">
         <v>328</v>
       </c>
+      <c r="I75" t="s" s="0">
+        <v>570</v>
+      </c>
       <c r="K75" t="s" s="0">
         <v>264</v>
       </c>
@@ -4920,6 +5427,9 @@
       <c r="H76" s="3" t="s">
         <v>329</v>
       </c>
+      <c r="I76" t="s" s="0">
+        <v>571</v>
+      </c>
       <c r="K76" t="s" s="0">
         <v>264</v>
       </c>
@@ -4962,7 +5472,10 @@
         <v>363</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>330</v>
+        <v>572</v>
+      </c>
+      <c r="I77" t="s" s="0">
+        <v>573</v>
       </c>
       <c r="K77" t="s" s="0">
         <v>264</v>
@@ -5014,6 +5527,9 @@
       <c r="H79" s="3" t="s">
         <v>331</v>
       </c>
+      <c r="I79" t="s" s="0">
+        <v>574</v>
+      </c>
       <c r="K79" t="s" s="0">
         <v>264</v>
       </c>
@@ -5056,7 +5572,10 @@
         <v>363</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>332</v>
+        <v>575</v>
+      </c>
+      <c r="I80" t="s" s="0">
+        <v>576</v>
       </c>
       <c r="K80" t="s" s="0">
         <v>264</v>
@@ -5102,6 +5621,9 @@
       <c r="H81" s="3" t="s">
         <v>333</v>
       </c>
+      <c r="I81" t="s" s="0">
+        <v>577</v>
+      </c>
       <c r="K81" t="s" s="0">
         <v>264</v>
       </c>
@@ -5146,6 +5668,9 @@
       <c r="H82" s="3" t="s">
         <v>334</v>
       </c>
+      <c r="I82" t="s" s="0">
+        <v>578</v>
+      </c>
       <c r="K82" t="s" s="0">
         <v>264</v>
       </c>
@@ -5188,7 +5713,10 @@
         <v>376</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>335</v>
+        <v>579</v>
+      </c>
+      <c r="I83" t="s" s="0">
+        <v>580</v>
       </c>
       <c r="K83" t="s" s="0">
         <v>264</v>
@@ -5230,6 +5758,9 @@
       </c>
       <c r="H84" s="3" t="s">
         <v>336</v>
+      </c>
+      <c r="I84" t="s" s="0">
+        <v>581</v>
       </c>
       <c r="K84" t="s" s="0">
         <v>264</v>
@@ -5281,6 +5812,9 @@
       <c r="H86" s="3" t="s">
         <v>337</v>
       </c>
+      <c r="I86" t="s" s="0">
+        <v>582</v>
+      </c>
       <c r="K86" t="s" s="0">
         <v>264</v>
       </c>
@@ -5325,6 +5859,9 @@
       <c r="H87" s="3" t="s">
         <v>338</v>
       </c>
+      <c r="I87" t="s" s="0">
+        <v>583</v>
+      </c>
       <c r="K87" t="s" s="0">
         <v>264</v>
       </c>
@@ -5369,6 +5906,9 @@
       <c r="H88" s="3" t="s">
         <v>339</v>
       </c>
+      <c r="I88" t="s" s="0">
+        <v>584</v>
+      </c>
       <c r="K88" t="s" s="0">
         <v>264</v>
       </c>
@@ -5413,6 +5953,9 @@
       <c r="H89" s="3" t="s">
         <v>340</v>
       </c>
+      <c r="I89" t="s" s="0">
+        <v>585</v>
+      </c>
       <c r="K89" t="s" s="0">
         <v>264</v>
       </c>
@@ -5454,6 +5997,9 @@
       <c r="H90" s="3" t="s">
         <v>341</v>
       </c>
+      <c r="I90" t="s" s="0">
+        <v>586</v>
+      </c>
       <c r="K90" t="s" s="0">
         <v>264</v>
       </c>
@@ -5498,6 +6044,9 @@
       <c r="H91" s="3" t="s">
         <v>342</v>
       </c>
+      <c r="I91" t="s" s="0">
+        <v>587</v>
+      </c>
       <c r="K91" t="s" s="0">
         <v>264</v>
       </c>
@@ -5542,6 +6091,9 @@
       <c r="H92" s="3" t="s">
         <v>343</v>
       </c>
+      <c r="I92" t="s" s="0">
+        <v>588</v>
+      </c>
       <c r="K92" t="s" s="0">
         <v>264</v>
       </c>
@@ -5586,6 +6138,9 @@
       <c r="H93" s="3" t="s">
         <v>344</v>
       </c>
+      <c r="I93" t="s" s="0">
+        <v>589</v>
+      </c>
       <c r="K93" t="s" s="0">
         <v>264</v>
       </c>
@@ -5628,6 +6183,9 @@
       <c r="H94" s="3" t="s">
         <v>345</v>
       </c>
+      <c r="I94" t="s" s="0">
+        <v>590</v>
+      </c>
       <c r="K94" t="s" s="0">
         <v>264</v>
       </c>
@@ -5671,6 +6229,9 @@
       </c>
       <c r="H95" s="3" t="s">
         <v>346</v>
+      </c>
+      <c r="I95" t="s" s="0">
+        <v>591</v>
       </c>
       <c r="K95" t="s" s="0">
         <v>264</v>
@@ -5750,7 +6311,10 @@
         <v>373</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>347</v>
+        <v>592</v>
+      </c>
+      <c r="I102" t="s" s="0">
+        <v>593</v>
       </c>
       <c r="K102" t="s" s="0">
         <v>264</v>
@@ -5794,7 +6358,10 @@
         <v>374</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>348</v>
+        <v>594</v>
+      </c>
+      <c r="I103" t="s" s="0">
+        <v>595</v>
       </c>
       <c r="K103" t="s" s="0">
         <v>264</v>
@@ -5840,6 +6407,9 @@
       <c r="H104" s="3" t="s">
         <v>349</v>
       </c>
+      <c r="I104" t="s" s="0">
+        <v>596</v>
+      </c>
       <c r="K104" t="s" s="0">
         <v>264</v>
       </c>
@@ -5884,6 +6454,9 @@
       <c r="H105" s="3" t="s">
         <v>350</v>
       </c>
+      <c r="I105" t="s" s="0">
+        <v>597</v>
+      </c>
       <c r="K105" t="s" s="0">
         <v>264</v>
       </c>
@@ -5926,7 +6499,10 @@
         <v>381</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>351</v>
+        <v>598</v>
+      </c>
+      <c r="I106" t="s" s="0">
+        <v>599</v>
       </c>
       <c r="K106" t="s" s="0">
         <v>264</v>
@@ -6092,6 +6668,9 @@
       <c r="H127" s="3" t="s">
         <v>352</v>
       </c>
+      <c r="I127" t="s" s="0">
+        <v>600</v>
+      </c>
       <c r="K127" t="s" s="0">
         <v>264</v>
       </c>
@@ -6134,7 +6713,10 @@
         <v>369</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>353</v>
+        <v>601</v>
+      </c>
+      <c r="I128" t="s" s="0">
+        <v>602</v>
       </c>
       <c r="K128" t="s" s="0">
         <v>264</v>
@@ -6180,6 +6762,9 @@
       <c r="H129" s="3" t="s">
         <v>354</v>
       </c>
+      <c r="I129" t="s" s="0">
+        <v>603</v>
+      </c>
       <c r="K129" t="s" s="0">
         <v>264</v>
       </c>
@@ -6224,6 +6809,9 @@
       <c r="H130" s="3" t="s">
         <v>355</v>
       </c>
+      <c r="I130" t="s" s="0">
+        <v>604</v>
+      </c>
       <c r="K130" t="s" s="0">
         <v>264</v>
       </c>
@@ -6268,6 +6856,9 @@
       <c r="H131" s="3" t="s">
         <v>356</v>
       </c>
+      <c r="I131" t="s" s="0">
+        <v>605</v>
+      </c>
       <c r="K131" t="s" s="0">
         <v>264</v>
       </c>
@@ -6312,6 +6903,9 @@
       <c r="H132" s="3" t="s">
         <v>357</v>
       </c>
+      <c r="I132" t="s" s="0">
+        <v>606</v>
+      </c>
       <c r="K132" t="s" s="0">
         <v>264</v>
       </c>
@@ -6356,6 +6950,9 @@
       <c r="H133" s="3" t="s">
         <v>358</v>
       </c>
+      <c r="I133" t="s" s="0">
+        <v>607</v>
+      </c>
       <c r="K133" t="s" s="0">
         <v>264</v>
       </c>
@@ -6400,6 +6997,9 @@
       <c r="H134" s="3" t="s">
         <v>359</v>
       </c>
+      <c r="I134" t="s" s="0">
+        <v>608</v>
+      </c>
       <c r="K134" t="s" s="0">
         <v>264</v>
       </c>
@@ -6442,6 +7042,9 @@
       <c r="H135" s="3" t="s">
         <v>360</v>
       </c>
+      <c r="I135" t="s" s="0">
+        <v>609</v>
+      </c>
       <c r="K135" t="s" s="0">
         <v>264</v>
       </c>
@@ -6485,6 +7088,9 @@
       </c>
       <c r="H136" s="3" t="s">
         <v>361</v>
+      </c>
+      <c r="I136" t="s" s="0">
+        <v>610</v>
       </c>
       <c r="K136" t="s" s="0">
         <v>264</v>

</xml_diff>

<commit_message>
Empezada Practica VI: Metodo para obtener las ordenanzas en el excel completado. Creacion de objetos para generar el xml
</commit_message>
<xml_diff>
--- a/resources/SistemasAgua.xlsx
+++ b/resources/SistemasAgua.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hds_8\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CDCD2C-2EAC-4C61-BE5E-27C5B0C01D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA42F524-A6D0-442B-A471-5D24016F1AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="611">
   <si>
     <t>Nombre</t>
   </si>
@@ -7183,7 +7183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A8F51-8D2A-4E56-BAC3-F686CC936FAB}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implementado correctamente tramos acumulables
</commit_message>
<xml_diff>
--- a/resources/SistemasAgua.xlsx
+++ b/resources/SistemasAgua.xlsx
@@ -5,39 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hds_8\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\202898\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA42F524-A6D0-442B-A471-5D24016F1AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FF753A-F146-4478-9E33-87A6307BEA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Contribuyente" sheetId="1" r:id="rId1"/>
     <sheet name="Ordenanza" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3021" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2515" uniqueCount="614">
   <si>
     <t>Nombre</t>
   </si>
@@ -1452,9 +1441,6 @@
     <t>Pueblo</t>
   </si>
   <si>
-    <t>Prueba</t>
-  </si>
-  <si>
     <t>Hogar</t>
   </si>
   <si>
@@ -1518,36 +1504,24 @@
     <t>SobreQueConcepto</t>
   </si>
   <si>
-    <t>Empresa</t>
-  </si>
-  <si>
     <t>conceptosACobrar</t>
   </si>
   <si>
     <t>1 2 3</t>
   </si>
   <si>
-    <t>1 2</t>
-  </si>
-  <si>
     <t>TipoCalculo</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Importe Desagüe</t>
   </si>
   <si>
     <t>Juan</t>
   </si>
   <si>
-    <t>3 1</t>
-  </si>
-  <si>
     <t>PYME</t>
   </si>
   <si>
@@ -1555,6 +1529,30 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Astorga</t>
+  </si>
+  <si>
+    <t>Cuarto tramo</t>
+  </si>
+  <si>
+    <t>Agua cuarto tramo</t>
+  </si>
+  <si>
+    <t>Gran empresa</t>
+  </si>
+  <si>
+    <t>Precio fijo alcantarillado</t>
+  </si>
+  <si>
+    <t>Importe alcantarillado</t>
+  </si>
+  <si>
+    <t>4 5 10</t>
+  </si>
+  <si>
+    <t>6 8 9</t>
   </si>
   <si>
     <t>DK7331645124473461205164</t>
@@ -1948,9 +1946,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1988,7 +1986,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2094,7 +2092,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2236,7 +2234,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2246,22 +2244,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6ACB8-7F34-425E-9257-91AD8B97F35F}">
   <dimension ref="A1:Q152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q60" sqref="Q60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="30.109375"/>
-    <col min="6" max="6" customWidth="true" style="5" width="30.109375"/>
-    <col min="8" max="8" customWidth="true" width="22.5546875"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.88671875"/>
+    <col min="5" max="5" customWidth="true" width="30.140625"/>
+    <col min="6" max="6" customWidth="true" style="5" width="30.140625"/>
+    <col min="8" max="8" customWidth="true" width="22.5703125"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.85546875"/>
     <col min="14" max="14" customWidth="true" width="14.0"/>
-    <col min="15" max="15" style="7" width="11.44140625"/>
-    <col min="17" max="17" style="1" width="11.44140625"/>
+    <col min="15" max="15" style="7" width="11.42578125"/>
+    <col min="17" max="17" style="1" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -2311,12 +2309,12 @@
         <v>266</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>95</v>
@@ -2340,10 +2338,10 @@
         <v>267</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>264</v>
+        <v>500</v>
       </c>
       <c r="L2" s="0">
         <v>0</v>
@@ -2358,10 +2356,10 @@
         <v>45294</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
         <v>14</v>
       </c>
@@ -2387,7 +2385,7 @@
         <v>268</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="K3" t="s" s="0">
         <v>264</v>
@@ -2405,10 +2403,10 @@
         <v>38267</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
         <v>15</v>
       </c>
@@ -2434,7 +2432,7 @@
         <v>269</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="K4" t="s" s="0">
         <v>264</v>
@@ -2452,10 +2450,10 @@
         <v>39682</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="0">
         <v>15</v>
       </c>
@@ -2481,13 +2479,13 @@
         <v>270</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="K5" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L5" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M5" s="0">
         <v>942</v>
@@ -2499,10 +2497,10 @@
         <v>38765</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s" s="0">
         <v>16</v>
       </c>
@@ -2528,7 +2526,7 @@
         <v>271</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="K6" t="s" s="0">
         <v>264</v>
@@ -2546,10 +2544,10 @@
         <v>38646</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s" s="0">
         <v>17</v>
       </c>
@@ -2575,7 +2573,7 @@
         <v>272</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="K7" t="s" s="0">
         <v>264</v>
@@ -2593,10 +2591,10 @@
         <v>41039</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s" s="0">
         <v>18</v>
       </c>
@@ -2622,13 +2620,13 @@
         <v>273</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="K8" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L8" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M8" s="0">
         <v>586</v>
@@ -2640,10 +2638,10 @@
         <v>43912</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s" s="0">
         <v>18</v>
       </c>
@@ -2669,7 +2667,7 @@
         <v>274</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="K9" t="s" s="0">
         <v>264</v>
@@ -2687,10 +2685,10 @@
         <v>41745</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s" s="0">
         <v>19</v>
       </c>
@@ -2716,7 +2714,7 @@
         <v>275</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="K10" t="s" s="0">
         <v>264</v>
@@ -2734,10 +2732,10 @@
         <v>44978</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s" s="0">
         <v>20</v>
       </c>
@@ -2763,13 +2761,13 @@
         <v>276</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="K11" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L11" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M11" s="0">
         <v>645</v>
@@ -2781,10 +2779,10 @@
         <v>39134</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s" s="0">
         <v>21</v>
       </c>
@@ -2810,7 +2808,7 @@
         <v>277</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="K12" t="s" s="0">
         <v>264</v>
@@ -2828,10 +2826,10 @@
         <v>44614</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s" s="0">
         <v>22</v>
       </c>
@@ -2857,7 +2855,7 @@
         <v>278</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="K13" t="s" s="0">
         <v>264</v>
@@ -2875,10 +2873,10 @@
         <v>41490</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s" s="0">
         <v>23</v>
       </c>
@@ -2904,13 +2902,13 @@
         <v>279</v>
       </c>
       <c r="I14" t="s" s="0">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="K14" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L14" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M14" s="0">
         <v>72</v>
@@ -2922,16 +2920,16 @@
         <v>41228</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s" s="0">
         <v>24</v>
       </c>
@@ -2957,7 +2955,7 @@
         <v>280</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="K16" t="s" s="0">
         <v>264</v>
@@ -2975,10 +2973,10 @@
         <v>40637</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s" s="0">
         <v>25</v>
       </c>
@@ -3004,7 +3002,7 @@
         <v>281</v>
       </c>
       <c r="I17" t="s" s="0">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="K17" t="s" s="0">
         <v>264</v>
@@ -3022,10 +3020,10 @@
         <v>45079</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s" s="0">
         <v>26</v>
       </c>
@@ -3036,7 +3034,7 @@
         <v>144</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>393</v>
@@ -3051,7 +3049,7 @@
         <v>282</v>
       </c>
       <c r="I18" t="s" s="0">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="K18" t="s" s="0">
         <v>264</v>
@@ -3069,10 +3067,10 @@
         <v>43017</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s" s="0">
         <v>27</v>
       </c>
@@ -3098,13 +3096,13 @@
         <v>283</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="K19" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L19" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M19" s="0">
         <v>968</v>
@@ -3116,10 +3114,10 @@
         <v>39371</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s" s="0">
         <v>28</v>
       </c>
@@ -3145,7 +3143,7 @@
         <v>284</v>
       </c>
       <c r="I20" t="s" s="0">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="K20" t="s" s="0">
         <v>264</v>
@@ -3163,10 +3161,10 @@
         <v>39934</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s" s="0">
         <v>29</v>
       </c>
@@ -3192,7 +3190,7 @@
         <v>279</v>
       </c>
       <c r="I21" t="s" s="0">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="K21" t="s" s="0">
         <v>264</v>
@@ -3210,10 +3208,10 @@
         <v>43868</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s" s="0">
         <v>30</v>
       </c>
@@ -3236,13 +3234,13 @@
         <v>285</v>
       </c>
       <c r="I22" t="s" s="0">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="K22" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L22" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M22" s="0">
         <v>25</v>
@@ -3254,10 +3252,10 @@
         <v>41262</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s" s="0">
         <v>31</v>
       </c>
@@ -3280,7 +3278,7 @@
         <v>286</v>
       </c>
       <c r="I23" t="s" s="0">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="K23" t="s" s="0">
         <v>264</v>
@@ -3298,10 +3296,10 @@
         <v>45279</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s" s="0">
         <v>32</v>
       </c>
@@ -3324,7 +3322,7 @@
         <v>287</v>
       </c>
       <c r="I24" t="s" s="0">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="K24" t="s" s="0">
         <v>264</v>
@@ -3342,10 +3340,10 @@
         <v>39982</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s" s="0">
         <v>33</v>
       </c>
@@ -3368,13 +3366,13 @@
         <v>288</v>
       </c>
       <c r="I25" t="s" s="0">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="K25" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L25" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M25" s="0">
         <v>799</v>
@@ -3386,16 +3384,16 @@
         <v>41034</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s" s="0">
         <v>34</v>
       </c>
@@ -3421,7 +3419,7 @@
         <v>289</v>
       </c>
       <c r="I27" t="s" s="0">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="K27" t="s" s="0">
         <v>264</v>
@@ -3439,10 +3437,10 @@
         <v>39525</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s" s="0">
         <v>35</v>
       </c>
@@ -3468,13 +3466,13 @@
         <v>290</v>
       </c>
       <c r="I28" t="s" s="0">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="K28" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L28" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M28" s="0">
         <v>410</v>
@@ -3486,10 +3484,10 @@
         <v>42667</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s" s="0">
         <v>36</v>
       </c>
@@ -3515,7 +3513,7 @@
         <v>291</v>
       </c>
       <c r="I29" t="s" s="0">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="K29" t="s" s="0">
         <v>264</v>
@@ -3533,10 +3531,10 @@
         <v>44639</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s" s="0">
         <v>37</v>
       </c>
@@ -3562,7 +3560,7 @@
         <v>292</v>
       </c>
       <c r="I30" t="s" s="0">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="K30" t="s" s="0">
         <v>264</v>
@@ -3580,10 +3578,10 @@
         <v>37937</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s" s="0">
         <v>38</v>
       </c>
@@ -3609,7 +3607,7 @@
         <v>293</v>
       </c>
       <c r="I31" t="s" s="0">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="K31" t="s" s="0">
         <v>264</v>
@@ -3627,10 +3625,10 @@
         <v>43242</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s" s="0">
         <v>39</v>
       </c>
@@ -3656,7 +3654,7 @@
         <v>294</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="K32" t="s" s="0">
         <v>264</v>
@@ -3674,28 +3672,28 @@
         <v>39555</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s" s="0">
         <v>40</v>
       </c>
@@ -3721,13 +3719,13 @@
         <v>295</v>
       </c>
       <c r="I36" t="s" s="0">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="K36" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L36" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M36" s="0">
         <v>413</v>
@@ -3739,10 +3737,10 @@
         <v>43230</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s" s="0">
         <v>41</v>
       </c>
@@ -3768,7 +3766,7 @@
         <v>296</v>
       </c>
       <c r="I37" t="s" s="0">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="K37" t="s" s="0">
         <v>264</v>
@@ -3786,10 +3784,10 @@
         <v>38841</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s" s="0">
         <v>42</v>
       </c>
@@ -3815,7 +3813,7 @@
         <v>297</v>
       </c>
       <c r="I38" t="s" s="0">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="K38" t="s" s="0">
         <v>264</v>
@@ -3833,10 +3831,10 @@
         <v>44389</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s" s="0">
         <v>43</v>
       </c>
@@ -3862,7 +3860,7 @@
         <v>298</v>
       </c>
       <c r="I39" t="s" s="0">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="K39" t="s" s="0">
         <v>264</v>
@@ -3880,10 +3878,10 @@
         <v>45242</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s" s="0">
         <v>44</v>
       </c>
@@ -3909,7 +3907,7 @@
         <v>299</v>
       </c>
       <c r="I40" t="s" s="0">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="K40" t="s" s="0">
         <v>264</v>
@@ -3927,10 +3925,10 @@
         <v>41309</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s" s="0">
         <v>45</v>
       </c>
@@ -3956,7 +3954,7 @@
         <v>300</v>
       </c>
       <c r="I41" t="s" s="0">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="K41" t="s" s="0">
         <v>264</v>
@@ -3974,10 +3972,10 @@
         <v>45142</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s" s="0">
         <v>46</v>
       </c>
@@ -4003,7 +4001,7 @@
         <v>301</v>
       </c>
       <c r="I42" t="s" s="0">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="K42" t="s" s="0">
         <v>264</v>
@@ -4021,10 +4019,10 @@
         <v>45048</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s" s="0">
         <v>47</v>
       </c>
@@ -4050,7 +4048,7 @@
         <v>302</v>
       </c>
       <c r="I43" t="s" s="0">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="K43" t="s" s="0">
         <v>264</v>
@@ -4068,10 +4066,10 @@
         <v>44479</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s" s="0">
         <v>39</v>
       </c>
@@ -4097,7 +4095,7 @@
         <v>303</v>
       </c>
       <c r="I44" t="s" s="0">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="K44" t="s" s="0">
         <v>264</v>
@@ -4115,10 +4113,10 @@
         <v>42624</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s" s="0">
         <v>48</v>
       </c>
@@ -4144,7 +4142,7 @@
         <v>304</v>
       </c>
       <c r="I45" t="s" s="0">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="K45" t="s" s="0">
         <v>264</v>
@@ -4162,10 +4160,10 @@
         <v>42708</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s" s="0">
         <v>49</v>
       </c>
@@ -4191,7 +4189,7 @@
         <v>305</v>
       </c>
       <c r="I46" t="s" s="0">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="K46" t="s" s="0">
         <v>264</v>
@@ -4209,10 +4207,10 @@
         <v>44180</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s" s="0">
         <v>50</v>
       </c>
@@ -4238,7 +4236,7 @@
         <v>306</v>
       </c>
       <c r="I47" t="s" s="0">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="K47" t="s" s="0">
         <v>264</v>
@@ -4256,10 +4254,10 @@
         <v>45047</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s" s="0">
         <v>51</v>
       </c>
@@ -4285,13 +4283,13 @@
         <v>286</v>
       </c>
       <c r="I48" t="s" s="0">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="K48" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L48" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M48" s="0">
         <v>330</v>
@@ -4303,10 +4301,10 @@
         <v>42182</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s" s="0">
         <v>52</v>
       </c>
@@ -4332,7 +4330,7 @@
         <v>307</v>
       </c>
       <c r="I49" t="s" s="0">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="K49" t="s" s="0">
         <v>264</v>
@@ -4350,10 +4348,10 @@
         <v>43032</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s" s="0">
         <v>53</v>
       </c>
@@ -4379,7 +4377,7 @@
         <v>308</v>
       </c>
       <c r="I50" t="s" s="0">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="K50" t="s" s="0">
         <v>264</v>
@@ -4397,10 +4395,10 @@
         <v>42490</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s" s="0">
         <v>53</v>
       </c>
@@ -4426,13 +4424,13 @@
         <v>309</v>
       </c>
       <c r="I51" t="s" s="0">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="K51" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L51" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M51" s="0">
         <v>178</v>
@@ -4444,10 +4442,10 @@
         <v>39101</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s" s="0">
         <v>13</v>
       </c>
@@ -4473,7 +4471,7 @@
         <v>310</v>
       </c>
       <c r="I52" t="s" s="0">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="K52" t="s" s="0">
         <v>264</v>
@@ -4491,10 +4489,10 @@
         <v>44962</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s" s="0">
         <v>14</v>
       </c>
@@ -4520,7 +4518,7 @@
         <v>311</v>
       </c>
       <c r="I53" t="s" s="0">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="K53" t="s" s="0">
         <v>264</v>
@@ -4538,10 +4536,10 @@
         <v>42148</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s" s="0">
         <v>15</v>
       </c>
@@ -4567,13 +4565,13 @@
         <v>312</v>
       </c>
       <c r="I54" t="s" s="0">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="K54" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L54" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M54" s="0">
         <v>556</v>
@@ -4585,10 +4583,10 @@
         <v>43805</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s" s="0">
         <v>15</v>
       </c>
@@ -4614,7 +4612,7 @@
         <v>313</v>
       </c>
       <c r="I55" t="s" s="0">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="K55" t="s" s="0">
         <v>264</v>
@@ -4632,34 +4630,34 @@
         <v>40575</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="E56" s="4"/>
       <c r="F56" s="6"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="E57" s="4"/>
       <c r="F57" s="6"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="E58" s="4"/>
       <c r="F58" s="6"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="E59" s="4"/>
       <c r="F59" s="6"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s" s="0">
         <v>19</v>
       </c>
@@ -4685,7 +4683,7 @@
         <v>314</v>
       </c>
       <c r="I60" t="s" s="0">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="K60" t="s" s="0">
         <v>264</v>
@@ -4703,10 +4701,10 @@
         <v>38607</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s" s="0">
         <v>54</v>
       </c>
@@ -4732,7 +4730,7 @@
         <v>315</v>
       </c>
       <c r="I61" t="s" s="0">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="K61" t="s" s="0">
         <v>264</v>
@@ -4750,10 +4748,10 @@
         <v>42083</v>
       </c>
       <c r="Q61" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s" s="0">
         <v>21</v>
       </c>
@@ -4779,13 +4777,13 @@
         <v>316</v>
       </c>
       <c r="I62" t="s" s="0">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="K62" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L62" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M62" s="0">
         <v>446</v>
@@ -4797,10 +4795,10 @@
         <v>39105</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s" s="0">
         <v>22</v>
       </c>
@@ -4826,7 +4824,7 @@
         <v>317</v>
       </c>
       <c r="I63" t="s" s="0">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="K63" t="s" s="0">
         <v>264</v>
@@ -4844,10 +4842,10 @@
         <v>41938</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s" s="0">
         <v>23</v>
       </c>
@@ -4870,7 +4868,7 @@
         <v>318</v>
       </c>
       <c r="I64" t="s" s="0">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="K64" t="s" s="0">
         <v>264</v>
@@ -4888,10 +4886,10 @@
         <v>43691</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s" s="0">
         <v>55</v>
       </c>
@@ -4914,7 +4912,7 @@
         <v>319</v>
       </c>
       <c r="I65" t="s" s="0">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="K65" t="s" s="0">
         <v>264</v>
@@ -4932,10 +4930,10 @@
         <v>42810</v>
       </c>
       <c r="Q65" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s" s="0">
         <v>24</v>
       </c>
@@ -4958,7 +4956,7 @@
         <v>320</v>
       </c>
       <c r="I66" t="s" s="0">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="K66" t="s" s="0">
         <v>264</v>
@@ -4976,10 +4974,10 @@
         <v>45570</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s" s="0">
         <v>25</v>
       </c>
@@ -5005,7 +5003,7 @@
         <v>321</v>
       </c>
       <c r="I67" t="s" s="0">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="K67" t="s" s="0">
         <v>264</v>
@@ -5023,10 +5021,10 @@
         <v>40799</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s" s="0">
         <v>26</v>
       </c>
@@ -5052,7 +5050,7 @@
         <v>322</v>
       </c>
       <c r="I68" t="s" s="0">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="K68" t="s" s="0">
         <v>264</v>
@@ -5070,10 +5068,10 @@
         <v>42926</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s" s="0">
         <v>27</v>
       </c>
@@ -5099,13 +5097,13 @@
         <v>323</v>
       </c>
       <c r="I69" t="s" s="0">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="K69" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L69" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M69" s="0">
         <v>983</v>
@@ -5117,10 +5115,10 @@
         <v>43569</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s" s="0">
         <v>16</v>
       </c>
@@ -5146,7 +5144,7 @@
         <v>324</v>
       </c>
       <c r="I70" t="s" s="0">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="K70" t="s" s="0">
         <v>264</v>
@@ -5164,10 +5162,10 @@
         <v>42657</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s" s="0">
         <v>17</v>
       </c>
@@ -5193,7 +5191,7 @@
         <v>314</v>
       </c>
       <c r="I71" t="s" s="0">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="K71" t="s" s="0">
         <v>264</v>
@@ -5211,10 +5209,10 @@
         <v>38841</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s" s="0">
         <v>18</v>
       </c>
@@ -5240,7 +5238,7 @@
         <v>325</v>
       </c>
       <c r="I72" t="s" s="0">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K72" t="s" s="0">
         <v>264</v>
@@ -5258,10 +5256,10 @@
         <v>42522</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s" s="0">
         <v>18</v>
       </c>
@@ -5287,7 +5285,7 @@
         <v>326</v>
       </c>
       <c r="I73" t="s" s="0">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="K73" t="s" s="0">
         <v>264</v>
@@ -5305,10 +5303,10 @@
         <v>39748</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s" s="0">
         <v>56</v>
       </c>
@@ -5334,13 +5332,13 @@
         <v>327</v>
       </c>
       <c r="I74" t="s" s="0">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="K74" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L74" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M74" s="0">
         <v>545</v>
@@ -5352,10 +5350,10 @@
         <v>40427</v>
       </c>
       <c r="Q74" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s" s="0">
         <v>57</v>
       </c>
@@ -5381,7 +5379,7 @@
         <v>328</v>
       </c>
       <c r="I75" t="s" s="0">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="K75" t="s" s="0">
         <v>264</v>
@@ -5399,10 +5397,10 @@
         <v>42543</v>
       </c>
       <c r="Q75" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s" s="0">
         <v>58</v>
       </c>
@@ -5428,7 +5426,7 @@
         <v>329</v>
       </c>
       <c r="I76" t="s" s="0">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="K76" t="s" s="0">
         <v>264</v>
@@ -5446,10 +5444,10 @@
         <v>45341</v>
       </c>
       <c r="Q76" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s" s="0">
         <v>59</v>
       </c>
@@ -5472,10 +5470,10 @@
         <v>363</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="I77" t="s" s="0">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="K77" t="s" s="0">
         <v>264</v>
@@ -5493,16 +5491,16 @@
         <v>39295</v>
       </c>
       <c r="Q77" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D78" s="1"/>
       <c r="E78" s="4"/>
       <c r="F78" s="6"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s" s="0">
         <v>60</v>
       </c>
@@ -5528,7 +5526,7 @@
         <v>331</v>
       </c>
       <c r="I79" t="s" s="0">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="K79" t="s" s="0">
         <v>264</v>
@@ -5546,10 +5544,10 @@
         <v>38315</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s" s="0">
         <v>61</v>
       </c>
@@ -5572,16 +5570,16 @@
         <v>363</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="I80" t="s" s="0">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="K80" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L80" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M80" s="0">
         <v>692</v>
@@ -5593,10 +5591,10 @@
         <v>43991</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s" s="0">
         <v>62</v>
       </c>
@@ -5622,7 +5620,7 @@
         <v>333</v>
       </c>
       <c r="I81" t="s" s="0">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="K81" t="s" s="0">
         <v>264</v>
@@ -5640,10 +5638,10 @@
         <v>45030</v>
       </c>
       <c r="Q81" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s" s="0">
         <v>63</v>
       </c>
@@ -5669,7 +5667,7 @@
         <v>334</v>
       </c>
       <c r="I82" t="s" s="0">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="K82" t="s" s="0">
         <v>264</v>
@@ -5687,10 +5685,10 @@
         <v>40558</v>
       </c>
       <c r="Q82" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s" s="0">
         <v>64</v>
       </c>
@@ -5713,10 +5711,10 @@
         <v>376</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="I83" t="s" s="0">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="K83" t="s" s="0">
         <v>264</v>
@@ -5734,10 +5732,10 @@
         <v>42650</v>
       </c>
       <c r="Q83" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s" s="0">
         <v>65</v>
       </c>
@@ -5760,7 +5758,7 @@
         <v>336</v>
       </c>
       <c r="I84" t="s" s="0">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="K84" t="s" s="0">
         <v>264</v>
@@ -5778,16 +5776,16 @@
         <v>41024</v>
       </c>
       <c r="Q84" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D85" s="1"/>
       <c r="E85" s="4"/>
       <c r="F85" s="6"/>
       <c r="H85" s="3"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s" s="0">
         <v>66</v>
       </c>
@@ -5813,13 +5811,13 @@
         <v>337</v>
       </c>
       <c r="I86" t="s" s="0">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="K86" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L86" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M86" s="0">
         <v>597</v>
@@ -5831,10 +5829,10 @@
         <v>45627</v>
       </c>
       <c r="Q86" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s" s="0">
         <v>67</v>
       </c>
@@ -5860,7 +5858,7 @@
         <v>338</v>
       </c>
       <c r="I87" t="s" s="0">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="K87" t="s" s="0">
         <v>264</v>
@@ -5878,10 +5876,10 @@
         <v>39308</v>
       </c>
       <c r="Q87" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s" s="0">
         <v>68</v>
       </c>
@@ -5907,7 +5905,7 @@
         <v>339</v>
       </c>
       <c r="I88" t="s" s="0">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="K88" t="s" s="0">
         <v>264</v>
@@ -5925,10 +5923,10 @@
         <v>40028</v>
       </c>
       <c r="Q88" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s" s="0">
         <v>69</v>
       </c>
@@ -5954,7 +5952,7 @@
         <v>340</v>
       </c>
       <c r="I89" t="s" s="0">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="K89" t="s" s="0">
         <v>264</v>
@@ -5972,10 +5970,10 @@
         <v>39734</v>
       </c>
       <c r="Q89" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s" s="0">
         <v>52</v>
       </c>
@@ -5998,7 +5996,7 @@
         <v>341</v>
       </c>
       <c r="I90" t="s" s="0">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="K90" t="s" s="0">
         <v>264</v>
@@ -6016,10 +6014,10 @@
         <v>40418</v>
       </c>
       <c r="Q90" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s" s="0">
         <v>70</v>
       </c>
@@ -6045,7 +6043,7 @@
         <v>342</v>
       </c>
       <c r="I91" t="s" s="0">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="K91" t="s" s="0">
         <v>264</v>
@@ -6063,10 +6061,10 @@
         <v>39480</v>
       </c>
       <c r="Q91" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s" s="0">
         <v>71</v>
       </c>
@@ -6092,7 +6090,7 @@
         <v>343</v>
       </c>
       <c r="I92" t="s" s="0">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="K92" t="s" s="0">
         <v>264</v>
@@ -6110,10 +6108,10 @@
         <v>39939</v>
       </c>
       <c r="Q92" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" t="s" s="0">
         <v>72</v>
       </c>
@@ -6139,13 +6137,13 @@
         <v>344</v>
       </c>
       <c r="I93" t="s" s="0">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K93" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L93" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M93" s="0">
         <v>76</v>
@@ -6157,10 +6155,10 @@
         <v>41007</v>
       </c>
       <c r="Q93" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s" s="0">
         <v>73</v>
       </c>
@@ -6184,7 +6182,7 @@
         <v>345</v>
       </c>
       <c r="I94" t="s" s="0">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="K94" t="s" s="0">
         <v>264</v>
@@ -6202,10 +6200,10 @@
         <v>41247</v>
       </c>
       <c r="Q94" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s" s="0">
         <v>74</v>
       </c>
@@ -6231,7 +6229,7 @@
         <v>346</v>
       </c>
       <c r="I95" t="s" s="0">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="K95" t="s" s="0">
         <v>264</v>
@@ -6249,46 +6247,46 @@
         <v>45099</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D96" s="1"/>
       <c r="E96" s="4"/>
       <c r="F96" s="6"/>
       <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D97" s="1"/>
       <c r="E97" s="4"/>
       <c r="F97" s="6"/>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D98" s="1"/>
       <c r="E98" s="4"/>
       <c r="F98" s="6"/>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D99" s="1"/>
       <c r="E99" s="4"/>
       <c r="F99" s="6"/>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D100" s="1"/>
       <c r="E100" s="4"/>
       <c r="F100" s="6"/>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D101" s="1"/>
       <c r="E101" s="4"/>
       <c r="F101" s="6"/>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s" s="0">
         <v>56</v>
       </c>
@@ -6311,10 +6309,10 @@
         <v>373</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="I102" t="s" s="0">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="K102" t="s" s="0">
         <v>264</v>
@@ -6332,10 +6330,10 @@
         <v>40726</v>
       </c>
       <c r="Q102" s="1" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s" s="0">
         <v>57</v>
       </c>
@@ -6358,16 +6356,16 @@
         <v>374</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="I103" t="s" s="0">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="K103" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L103" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M103" s="0">
         <v>964</v>
@@ -6379,10 +6377,10 @@
         <v>44937</v>
       </c>
       <c r="Q103" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s" s="0">
         <v>58</v>
       </c>
@@ -6408,7 +6406,7 @@
         <v>349</v>
       </c>
       <c r="I104" t="s" s="0">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="K104" t="s" s="0">
         <v>264</v>
@@ -6426,10 +6424,10 @@
         <v>40195</v>
       </c>
       <c r="Q104" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s" s="0">
         <v>59</v>
       </c>
@@ -6455,7 +6453,7 @@
         <v>350</v>
       </c>
       <c r="I105" t="s" s="0">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="K105" t="s" s="0">
         <v>264</v>
@@ -6473,10 +6471,10 @@
         <v>40974</v>
       </c>
       <c r="Q105" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s" s="0">
         <v>13</v>
       </c>
@@ -6499,16 +6497,16 @@
         <v>381</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="I106" t="s" s="0">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="K106" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L106" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M106" s="0">
         <v>188</v>
@@ -6520,130 +6518,130 @@
         <v>44615</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D107" s="1"/>
       <c r="E107" s="4"/>
       <c r="F107" s="6"/>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D108" s="1"/>
       <c r="E108" s="4"/>
       <c r="F108" s="6"/>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D109" s="1"/>
       <c r="E109" s="4"/>
       <c r="F109" s="6"/>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D110" s="1"/>
       <c r="E110" s="4"/>
       <c r="F110" s="6"/>
       <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D111" s="1"/>
       <c r="E111" s="4"/>
       <c r="F111" s="6"/>
       <c r="H111" s="3"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D112" s="1"/>
       <c r="E112" s="4"/>
       <c r="F112" s="6"/>
       <c r="H112" s="3"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D113" s="1"/>
       <c r="E113" s="4"/>
       <c r="F113" s="6"/>
       <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D114" s="1"/>
       <c r="E114" s="4"/>
       <c r="F114" s="6"/>
       <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D115" s="1"/>
       <c r="E115" s="4"/>
       <c r="F115" s="6"/>
       <c r="H115" s="3"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D116" s="1"/>
       <c r="E116" s="4"/>
       <c r="F116" s="6"/>
       <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D117" s="1"/>
       <c r="E117" s="4"/>
       <c r="F117" s="6"/>
       <c r="H117" s="3"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D118" s="1"/>
       <c r="E118" s="4"/>
       <c r="F118" s="6"/>
       <c r="H118" s="3"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D119" s="1"/>
       <c r="E119" s="4"/>
       <c r="F119" s="6"/>
       <c r="H119" s="3"/>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D120" s="1"/>
       <c r="E120" s="4"/>
       <c r="F120" s="6"/>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D121" s="1"/>
       <c r="E121" s="4"/>
       <c r="F121" s="6"/>
       <c r="H121" s="3"/>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D122" s="1"/>
       <c r="E122" s="4"/>
       <c r="F122" s="6"/>
       <c r="H122" s="3"/>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D123" s="1"/>
       <c r="E123" s="4"/>
       <c r="F123" s="6"/>
       <c r="H123" s="3"/>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D124" s="1"/>
       <c r="E124" s="4"/>
       <c r="F124" s="6"/>
       <c r="H124" s="3"/>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D125" s="1"/>
       <c r="E125" s="4"/>
       <c r="F125" s="6"/>
       <c r="H125" s="3"/>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D126" s="1"/>
       <c r="E126" s="4"/>
       <c r="F126" s="6"/>
       <c r="H126" s="3"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" t="s" s="0">
         <v>75</v>
       </c>
@@ -6669,7 +6667,7 @@
         <v>352</v>
       </c>
       <c r="I127" t="s" s="0">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="K127" t="s" s="0">
         <v>264</v>
@@ -6687,10 +6685,10 @@
         <v>39738</v>
       </c>
       <c r="Q127" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" t="s" s="0">
         <v>76</v>
       </c>
@@ -6713,10 +6711,10 @@
         <v>369</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="I128" t="s" s="0">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="K128" t="s" s="0">
         <v>264</v>
@@ -6734,10 +6732,10 @@
         <v>40453</v>
       </c>
       <c r="Q128" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s" s="0">
         <v>77</v>
       </c>
@@ -6763,7 +6761,7 @@
         <v>354</v>
       </c>
       <c r="I129" t="s" s="0">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="K129" t="s" s="0">
         <v>264</v>
@@ -6781,10 +6779,10 @@
         <v>43473</v>
       </c>
       <c r="Q129" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s" s="0">
         <v>68</v>
       </c>
@@ -6810,13 +6808,13 @@
         <v>355</v>
       </c>
       <c r="I130" t="s" s="0">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="K130" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L130" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M130" s="0">
         <v>1</v>
@@ -6828,10 +6826,10 @@
         <v>40935</v>
       </c>
       <c r="Q130" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" t="s" s="0">
         <v>69</v>
       </c>
@@ -6857,7 +6855,7 @@
         <v>356</v>
       </c>
       <c r="I131" t="s" s="0">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="K131" t="s" s="0">
         <v>264</v>
@@ -6875,10 +6873,10 @@
         <v>44175</v>
       </c>
       <c r="Q131" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" t="s" s="0">
         <v>52</v>
       </c>
@@ -6904,10 +6902,10 @@
         <v>357</v>
       </c>
       <c r="I132" t="s" s="0">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="K132" t="s" s="0">
-        <v>264</v>
+        <v>500</v>
       </c>
       <c r="L132" s="0">
         <v>0</v>
@@ -6922,10 +6920,10 @@
         <v>40887</v>
       </c>
       <c r="Q132" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" t="s" s="0">
         <v>70</v>
       </c>
@@ -6951,7 +6949,7 @@
         <v>358</v>
       </c>
       <c r="I133" t="s" s="0">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="K133" t="s" s="0">
         <v>264</v>
@@ -6969,10 +6967,10 @@
         <v>43334</v>
       </c>
       <c r="Q133" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" t="s" s="0">
         <v>71</v>
       </c>
@@ -6998,13 +6996,13 @@
         <v>359</v>
       </c>
       <c r="I134" t="s" s="0">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="K134" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L134" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M134" s="0">
         <v>728</v>
@@ -7016,10 +7014,10 @@
         <v>42557</v>
       </c>
       <c r="Q134" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" t="s" s="0">
         <v>72</v>
       </c>
@@ -7043,7 +7041,7 @@
         <v>360</v>
       </c>
       <c r="I135" t="s" s="0">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="K135" t="s" s="0">
         <v>264</v>
@@ -7061,10 +7059,10 @@
         <v>43929</v>
       </c>
       <c r="Q135" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" t="s" s="0">
         <v>73</v>
       </c>
@@ -7090,7 +7088,7 @@
         <v>361</v>
       </c>
       <c r="I136" t="s" s="0">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="K136" t="s" s="0">
         <v>264</v>
@@ -7108,69 +7106,69 @@
         <v>40457</v>
       </c>
       <c r="Q136" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E137" s="4"/>
       <c r="F137" s="6"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E138" s="4"/>
       <c r="F138" s="6"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E139" s="4"/>
       <c r="F139" s="6"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E140" s="4"/>
       <c r="F140" s="6"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E141" s="4"/>
       <c r="F141" s="6"/>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E142" s="4"/>
       <c r="F142" s="6"/>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E143" s="4"/>
       <c r="F143" s="6"/>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E144" s="4"/>
       <c r="F144" s="6"/>
     </row>
-    <row r="145" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E145" s="4"/>
       <c r="F145" s="6"/>
     </row>
-    <row r="146" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E146" s="4"/>
       <c r="F146" s="6"/>
     </row>
-    <row r="147" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E147" s="4"/>
       <c r="F147" s="6"/>
     </row>
-    <row r="148" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E148" s="4"/>
       <c r="F148" s="6"/>
     </row>
-    <row r="149" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E149" s="4"/>
       <c r="F149" s="6"/>
     </row>
-    <row r="150" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E150" s="4"/>
       <c r="F150" s="6"/>
     </row>
-    <row r="151" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F151" s="6"/>
     </row>
-    <row r="152" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F152" s="6"/>
     </row>
   </sheetData>
@@ -7181,80 +7179,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A8F51-8D2A-4E56-BAC3-F686CC936FAB}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.88671875"/>
-    <col min="2" max="2" customWidth="true" width="14.88671875"/>
+    <col min="1" max="1" customWidth="true" width="15.85546875"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875"/>
     <col min="6" max="6" customWidth="true" width="46.0"/>
-    <col min="7" max="7" customWidth="true" width="14.33203125"/>
-    <col min="11" max="12" customWidth="true" width="20.6640625"/>
+    <col min="7" max="7" customWidth="true" width="14.28515625"/>
+    <col min="11" max="12" customWidth="true" width="20.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="0">
         <v>470</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C1" t="s" s="0">
         <v>469</v>
       </c>
       <c r="D1" t="s" s="0">
+        <v>472</v>
+      </c>
+      <c r="E1" t="s" s="0">
         <v>473</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="F1" t="s" s="0">
         <v>474</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>475</v>
       </c>
       <c r="G1" t="s" s="0">
         <v>467</v>
       </c>
       <c r="H1" t="s" s="0">
+        <v>475</v>
+      </c>
+      <c r="I1" t="s" s="0">
         <v>476</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="J1" t="s" s="0">
         <v>477</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="K1" t="s" s="0">
         <v>478</v>
       </c>
-      <c r="K1" t="s" s="0">
-        <v>479</v>
-      </c>
       <c r="L1" t="s" s="0">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="M1" t="s" s="0">
         <v>468</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>471</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>472</v>
       </c>
       <c r="C2" s="0">
         <v>1</v>
       </c>
       <c r="D2" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>480</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="F2" t="s" s="0">
         <v>481</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>482</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>264</v>
@@ -7269,24 +7267,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>471</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>472</v>
       </c>
       <c r="C3" s="0">
         <v>1</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E3" t="s" s="0">
+        <v>482</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>483</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>484</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>264</v>
@@ -7301,24 +7299,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>471</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>472</v>
       </c>
       <c r="C4" s="0">
         <v>1</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E4" t="s" s="0">
+        <v>484</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>485</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>486</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>264</v>
@@ -7333,219 +7331,460 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>471</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>472</v>
       </c>
       <c r="C5" s="0">
         <v>1</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E5" t="s" s="0">
+        <v>486</v>
+      </c>
+      <c r="F5" t="s" s="0">
         <v>487</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>488</v>
-      </c>
       <c r="G5" t="s" s="0">
         <v>264</v>
       </c>
       <c r="I5" s="0">
-        <v>9999</v>
+        <v>100</v>
       </c>
       <c r="J5" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5" s="0">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>471</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>472</v>
-      </c>
       <c r="C6" s="0">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>502</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>503</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="I6" s="0">
+        <v>9999</v>
+      </c>
+      <c r="J6" s="0">
+        <v>5</v>
+      </c>
+      <c r="M6" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>471</v>
+      </c>
+      <c r="C7" s="0">
         <v>2</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D7" t="s" s="0">
+        <v>488</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="F7" t="s" s="0">
         <v>489</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>481</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="H6" s="0">
-        <v>12</v>
-      </c>
-      <c r="I6" s="0">
-        <v>0</v>
-      </c>
-      <c r="M6" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
-        <v>471</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>472</v>
-      </c>
-      <c r="C7" s="0">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>491</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>491</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>500</v>
       </c>
       <c r="K7" s="0">
         <v>10</v>
       </c>
       <c r="L7" s="0">
+        <v>3</v>
+      </c>
+      <c r="M7" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>471</v>
+      </c>
+      <c r="C8" s="0">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>496</v>
+      </c>
+      <c r="K8" s="0">
+        <v>10</v>
+      </c>
+      <c r="L8" s="0">
         <v>1</v>
       </c>
-      <c r="M7" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
-        <v>471</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>493</v>
-      </c>
-      <c r="C8" s="0">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>480</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>481</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>482</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>264</v>
-      </c>
-      <c r="H8" s="0">
-        <v>50</v>
-      </c>
-      <c r="I8" s="0">
-        <v>20</v>
-      </c>
       <c r="M8" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s" s="0">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="C9" s="0">
         <v>4</v>
       </c>
       <c r="D9" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E9" t="s" s="0">
         <v>480</v>
       </c>
-      <c r="E9" t="s" s="0">
-        <v>483</v>
-      </c>
       <c r="F9" t="s" s="0">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>264</v>
+        <v>500</v>
+      </c>
+      <c r="H9" s="0">
+        <v>50</v>
       </c>
       <c r="I9" s="0">
-        <v>9999</v>
-      </c>
-      <c r="J9" s="0">
-        <v>0.75</v>
+        <v>20</v>
       </c>
       <c r="M9" s="0">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s" s="0">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="C10" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="H10" s="0">
-        <v>25</v>
+        <v>483</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>500</v>
+      </c>
+      <c r="I10" s="0">
+        <v>50</v>
+      </c>
+      <c r="J10" s="0">
+        <v>1</v>
       </c>
       <c r="M10" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s" s="0">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C11" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>473</v>
+        <v>484</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>504</v>
+        <v>485</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>505</v>
-      </c>
-      <c r="H11" s="0">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="I11" s="0">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J11" s="0">
         <v>2</v>
       </c>
       <c r="M11" s="0">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="C12" s="0">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>486</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>487</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>500</v>
+      </c>
+      <c r="I12" s="0">
+        <v>100</v>
+      </c>
+      <c r="J12" s="0">
+        <v>5</v>
+      </c>
+      <c r="M12" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="C13" s="0">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>502</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>503</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>500</v>
+      </c>
+      <c r="I13" s="0">
+        <v>9999</v>
+      </c>
+      <c r="J13" s="0">
+        <v>10</v>
+      </c>
+      <c r="M13" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="C14" s="0">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>489</v>
+      </c>
+      <c r="H14" s="0">
+        <v>25</v>
+      </c>
+      <c r="M14" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>498</v>
+      </c>
+      <c r="C15" s="0">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>472</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>499</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>500</v>
+      </c>
+      <c r="H15" s="0">
+        <v>20</v>
+      </c>
+      <c r="I15" s="0">
+        <v>30</v>
+      </c>
+      <c r="J15" s="0">
+        <v>2</v>
+      </c>
+      <c r="M15" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>471</v>
+      </c>
+      <c r="C16" s="0">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>496</v>
+      </c>
+      <c r="K16" s="0">
+        <v>10</v>
+      </c>
+      <c r="L16" s="0">
+        <v>1</v>
+      </c>
+      <c r="M16" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>498</v>
+      </c>
+      <c r="C17" s="0">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>488</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>505</v>
+      </c>
+      <c r="H17" s="0">
+        <v>30</v>
+      </c>
+      <c r="M17" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>498</v>
+      </c>
+      <c r="C18" s="0">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>496</v>
+      </c>
+      <c r="K18" s="0">
+        <v>20</v>
+      </c>
+      <c r="L18" s="0">
+        <v>9</v>
+      </c>
+      <c r="M18" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="C19" s="0">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>488</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>506</v>
+      </c>
+      <c r="K19" s="0">
+        <v>10</v>
+      </c>
+      <c r="L19" s="0">
+        <v>4</v>
+      </c>
+      <c r="M19" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Falta arreglar errores genera recibos que no debe
</commit_message>
<xml_diff>
--- a/resources/SistemasAgua.xlsx
+++ b/resources/SistemasAgua.xlsx
@@ -5,28 +5,39 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\202898\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hds_8\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FF753A-F146-4478-9E33-87A6307BEA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA42F524-A6D0-442B-A471-5D24016F1AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Contribuyente" sheetId="1" r:id="rId1"/>
     <sheet name="Ordenanza" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9065" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="611">
   <si>
     <t>Nombre</t>
   </si>
@@ -1441,6 +1452,9 @@
     <t>Pueblo</t>
   </si>
   <si>
+    <t>Prueba</t>
+  </si>
+  <si>
     <t>Hogar</t>
   </si>
   <si>
@@ -1504,24 +1518,36 @@
     <t>SobreQueConcepto</t>
   </si>
   <si>
+    <t>Empresa</t>
+  </si>
+  <si>
     <t>conceptosACobrar</t>
   </si>
   <si>
     <t>1 2 3</t>
   </si>
   <si>
+    <t>1 2</t>
+  </si>
+  <si>
     <t>TipoCalculo</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Importe Desagüe</t>
   </si>
   <si>
     <t>Juan</t>
   </si>
   <si>
+    <t>3 1</t>
+  </si>
+  <si>
     <t>PYME</t>
   </si>
   <si>
@@ -1531,30 +1557,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>Astorga</t>
-  </si>
-  <si>
-    <t>Cuarto tramo</t>
-  </si>
-  <si>
-    <t>Agua cuarto tramo</t>
-  </si>
-  <si>
-    <t>Gran empresa</t>
-  </si>
-  <si>
-    <t>Precio fijo alcantarillado</t>
-  </si>
-  <si>
-    <t>Importe alcantarillado</t>
-  </si>
-  <si>
-    <t>4 5 10</t>
-  </si>
-  <si>
-    <t>6 8 9</t>
-  </si>
-  <si>
     <t>DK7331645124473461205164</t>
   </si>
   <si>
@@ -1600,10 +1602,10 @@
     <t>ES9596431245118150005156</t>
   </si>
   <si>
+    <t>AT6825030000114574745458</t>
+  </si>
+  <si>
     <t>09548416N</t>
-  </si>
-  <si>
-    <t>AT6825030000114574745458</t>
   </si>
   <si>
     <t>IT8915953684811254695203</t>
@@ -1946,9 +1948,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1986,7 +1988,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2092,7 +2094,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2234,7 +2236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2244,22 +2246,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6ACB8-7F34-425E-9257-91AD8B97F35F}">
   <dimension ref="A1:Q152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q60" sqref="Q60"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="30.140625"/>
-    <col min="6" max="6" customWidth="true" style="5" width="30.140625"/>
-    <col min="8" max="8" customWidth="true" width="22.5703125"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.85546875"/>
+    <col min="5" max="5" customWidth="true" width="30.109375"/>
+    <col min="6" max="6" customWidth="true" style="5" width="30.109375"/>
+    <col min="8" max="8" customWidth="true" width="22.5546875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.88671875"/>
     <col min="14" max="14" customWidth="true" width="14.0"/>
-    <col min="15" max="15" style="7" width="11.42578125"/>
-    <col min="17" max="17" style="1" width="11.42578125"/>
+    <col min="15" max="15" style="7" width="11.44140625"/>
+    <col min="17" max="17" style="1" width="11.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -2309,12 +2311,12 @@
         <v>266</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>95</v>
@@ -2338,10 +2340,10 @@
         <v>267</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>500</v>
+        <v>264</v>
       </c>
       <c r="L2" s="0">
         <v>0</v>
@@ -2356,10 +2358,10 @@
         <v>45294</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
         <v>14</v>
       </c>
@@ -2385,7 +2387,7 @@
         <v>268</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="K3" t="s" s="0">
         <v>264</v>
@@ -2403,10 +2405,10 @@
         <v>38267</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
         <v>15</v>
       </c>
@@ -2432,7 +2434,7 @@
         <v>269</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="K4" t="s" s="0">
         <v>264</v>
@@ -2450,10 +2452,10 @@
         <v>39682</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
         <v>15</v>
       </c>
@@ -2479,13 +2481,13 @@
         <v>270</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="K5" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L5" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M5" s="0">
         <v>942</v>
@@ -2497,10 +2499,10 @@
         <v>38765</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
         <v>16</v>
       </c>
@@ -2526,7 +2528,7 @@
         <v>271</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="K6" t="s" s="0">
         <v>264</v>
@@ -2544,10 +2546,10 @@
         <v>38646</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s" s="0">
         <v>17</v>
       </c>
@@ -2573,7 +2575,7 @@
         <v>272</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="K7" t="s" s="0">
         <v>264</v>
@@ -2591,10 +2593,10 @@
         <v>41039</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s" s="0">
         <v>18</v>
       </c>
@@ -2620,13 +2622,13 @@
         <v>273</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="K8" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L8" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M8" s="0">
         <v>586</v>
@@ -2638,10 +2640,10 @@
         <v>43912</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s" s="0">
         <v>18</v>
       </c>
@@ -2667,7 +2669,7 @@
         <v>274</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="K9" t="s" s="0">
         <v>264</v>
@@ -2685,10 +2687,10 @@
         <v>41745</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s" s="0">
         <v>19</v>
       </c>
@@ -2714,7 +2716,7 @@
         <v>275</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="K10" t="s" s="0">
         <v>264</v>
@@ -2732,10 +2734,10 @@
         <v>44978</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s" s="0">
         <v>20</v>
       </c>
@@ -2761,13 +2763,13 @@
         <v>276</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="K11" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L11" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M11" s="0">
         <v>645</v>
@@ -2779,10 +2781,10 @@
         <v>39134</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s" s="0">
         <v>21</v>
       </c>
@@ -2808,7 +2810,7 @@
         <v>277</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="K12" t="s" s="0">
         <v>264</v>
@@ -2826,10 +2828,10 @@
         <v>44614</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s" s="0">
         <v>22</v>
       </c>
@@ -2855,7 +2857,7 @@
         <v>278</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="K13" t="s" s="0">
         <v>264</v>
@@ -2873,10 +2875,10 @@
         <v>41490</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s" s="0">
         <v>23</v>
       </c>
@@ -2902,13 +2904,13 @@
         <v>279</v>
       </c>
       <c r="I14" t="s" s="0">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="K14" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L14" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M14" s="0">
         <v>72</v>
@@ -2920,16 +2922,16 @@
         <v>41228</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s" s="0">
         <v>24</v>
       </c>
@@ -2955,7 +2957,7 @@
         <v>280</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="K16" t="s" s="0">
         <v>264</v>
@@ -2973,10 +2975,10 @@
         <v>40637</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s" s="0">
         <v>25</v>
       </c>
@@ -3002,7 +3004,7 @@
         <v>281</v>
       </c>
       <c r="I17" t="s" s="0">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="K17" t="s" s="0">
         <v>264</v>
@@ -3020,10 +3022,10 @@
         <v>45079</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s" s="0">
         <v>26</v>
       </c>
@@ -3034,7 +3036,7 @@
         <v>144</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>393</v>
@@ -3049,7 +3051,7 @@
         <v>282</v>
       </c>
       <c r="I18" t="s" s="0">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="K18" t="s" s="0">
         <v>264</v>
@@ -3067,10 +3069,10 @@
         <v>43017</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s" s="0">
         <v>27</v>
       </c>
@@ -3096,13 +3098,13 @@
         <v>283</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="K19" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L19" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M19" s="0">
         <v>968</v>
@@ -3114,10 +3116,10 @@
         <v>39371</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s" s="0">
         <v>28</v>
       </c>
@@ -3143,7 +3145,7 @@
         <v>284</v>
       </c>
       <c r="I20" t="s" s="0">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="K20" t="s" s="0">
         <v>264</v>
@@ -3161,10 +3163,10 @@
         <v>39934</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s" s="0">
         <v>29</v>
       </c>
@@ -3190,7 +3192,7 @@
         <v>279</v>
       </c>
       <c r="I21" t="s" s="0">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="K21" t="s" s="0">
         <v>264</v>
@@ -3208,10 +3210,10 @@
         <v>43868</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s" s="0">
         <v>30</v>
       </c>
@@ -3234,13 +3236,13 @@
         <v>285</v>
       </c>
       <c r="I22" t="s" s="0">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="K22" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L22" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M22" s="0">
         <v>25</v>
@@ -3252,10 +3254,10 @@
         <v>41262</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s" s="0">
         <v>31</v>
       </c>
@@ -3278,7 +3280,7 @@
         <v>286</v>
       </c>
       <c r="I23" t="s" s="0">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="K23" t="s" s="0">
         <v>264</v>
@@ -3296,10 +3298,10 @@
         <v>45279</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s" s="0">
         <v>32</v>
       </c>
@@ -3322,7 +3324,7 @@
         <v>287</v>
       </c>
       <c r="I24" t="s" s="0">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="K24" t="s" s="0">
         <v>264</v>
@@ -3340,10 +3342,10 @@
         <v>39982</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s" s="0">
         <v>33</v>
       </c>
@@ -3366,13 +3368,13 @@
         <v>288</v>
       </c>
       <c r="I25" t="s" s="0">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="K25" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L25" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M25" s="0">
         <v>799</v>
@@ -3384,16 +3386,16 @@
         <v>41034</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D26" s="1"/>
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s" s="0">
         <v>34</v>
       </c>
@@ -3419,7 +3421,7 @@
         <v>289</v>
       </c>
       <c r="I27" t="s" s="0">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="K27" t="s" s="0">
         <v>264</v>
@@ -3437,10 +3439,10 @@
         <v>39525</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s" s="0">
         <v>35</v>
       </c>
@@ -3466,13 +3468,13 @@
         <v>290</v>
       </c>
       <c r="I28" t="s" s="0">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="K28" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L28" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M28" s="0">
         <v>410</v>
@@ -3484,10 +3486,10 @@
         <v>42667</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s" s="0">
         <v>36</v>
       </c>
@@ -3513,7 +3515,7 @@
         <v>291</v>
       </c>
       <c r="I29" t="s" s="0">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="K29" t="s" s="0">
         <v>264</v>
@@ -3531,10 +3533,10 @@
         <v>44639</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s" s="0">
         <v>37</v>
       </c>
@@ -3560,7 +3562,7 @@
         <v>292</v>
       </c>
       <c r="I30" t="s" s="0">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="K30" t="s" s="0">
         <v>264</v>
@@ -3578,10 +3580,10 @@
         <v>37937</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s" s="0">
         <v>38</v>
       </c>
@@ -3607,7 +3609,7 @@
         <v>293</v>
       </c>
       <c r="I31" t="s" s="0">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="K31" t="s" s="0">
         <v>264</v>
@@ -3625,10 +3627,10 @@
         <v>43242</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s" s="0">
         <v>39</v>
       </c>
@@ -3654,7 +3656,7 @@
         <v>294</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="K32" t="s" s="0">
         <v>264</v>
@@ -3672,28 +3674,28 @@
         <v>39555</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D33" s="1"/>
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D34" s="1"/>
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D35" s="1"/>
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" t="s" s="0">
         <v>40</v>
       </c>
@@ -3719,13 +3721,13 @@
         <v>295</v>
       </c>
       <c r="I36" t="s" s="0">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="K36" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L36" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M36" s="0">
         <v>413</v>
@@ -3737,10 +3739,10 @@
         <v>43230</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s" s="0">
         <v>41</v>
       </c>
@@ -3766,7 +3768,7 @@
         <v>296</v>
       </c>
       <c r="I37" t="s" s="0">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="K37" t="s" s="0">
         <v>264</v>
@@ -3784,10 +3786,10 @@
         <v>38841</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s" s="0">
         <v>42</v>
       </c>
@@ -3813,7 +3815,7 @@
         <v>297</v>
       </c>
       <c r="I38" t="s" s="0">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="K38" t="s" s="0">
         <v>264</v>
@@ -3831,10 +3833,10 @@
         <v>44389</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s" s="0">
         <v>43</v>
       </c>
@@ -3860,7 +3862,7 @@
         <v>298</v>
       </c>
       <c r="I39" t="s" s="0">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="K39" t="s" s="0">
         <v>264</v>
@@ -3878,10 +3880,10 @@
         <v>45242</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s" s="0">
         <v>44</v>
       </c>
@@ -3907,7 +3909,7 @@
         <v>299</v>
       </c>
       <c r="I40" t="s" s="0">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="K40" t="s" s="0">
         <v>264</v>
@@ -3925,10 +3927,10 @@
         <v>41309</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s" s="0">
         <v>45</v>
       </c>
@@ -3954,7 +3956,7 @@
         <v>300</v>
       </c>
       <c r="I41" t="s" s="0">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="K41" t="s" s="0">
         <v>264</v>
@@ -3972,10 +3974,10 @@
         <v>45142</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" t="s" s="0">
         <v>46</v>
       </c>
@@ -4001,7 +4003,7 @@
         <v>301</v>
       </c>
       <c r="I42" t="s" s="0">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="K42" t="s" s="0">
         <v>264</v>
@@ -4019,10 +4021,10 @@
         <v>45048</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s" s="0">
         <v>47</v>
       </c>
@@ -4048,7 +4050,7 @@
         <v>302</v>
       </c>
       <c r="I43" t="s" s="0">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="K43" t="s" s="0">
         <v>264</v>
@@ -4066,10 +4068,10 @@
         <v>44479</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" t="s" s="0">
         <v>39</v>
       </c>
@@ -4095,7 +4097,7 @@
         <v>303</v>
       </c>
       <c r="I44" t="s" s="0">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="K44" t="s" s="0">
         <v>264</v>
@@ -4113,10 +4115,10 @@
         <v>42624</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s" s="0">
         <v>48</v>
       </c>
@@ -4142,7 +4144,7 @@
         <v>304</v>
       </c>
       <c r="I45" t="s" s="0">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="K45" t="s" s="0">
         <v>264</v>
@@ -4160,10 +4162,10 @@
         <v>42708</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s" s="0">
         <v>49</v>
       </c>
@@ -4189,7 +4191,7 @@
         <v>305</v>
       </c>
       <c r="I46" t="s" s="0">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="K46" t="s" s="0">
         <v>264</v>
@@ -4207,10 +4209,10 @@
         <v>44180</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" t="s" s="0">
         <v>50</v>
       </c>
@@ -4236,7 +4238,7 @@
         <v>306</v>
       </c>
       <c r="I47" t="s" s="0">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="K47" t="s" s="0">
         <v>264</v>
@@ -4254,10 +4256,10 @@
         <v>45047</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s" s="0">
         <v>51</v>
       </c>
@@ -4283,13 +4285,13 @@
         <v>286</v>
       </c>
       <c r="I48" t="s" s="0">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="K48" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L48" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M48" s="0">
         <v>330</v>
@@ -4301,10 +4303,10 @@
         <v>42182</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" t="s" s="0">
         <v>52</v>
       </c>
@@ -4330,7 +4332,7 @@
         <v>307</v>
       </c>
       <c r="I49" t="s" s="0">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="K49" t="s" s="0">
         <v>264</v>
@@ -4348,10 +4350,10 @@
         <v>43032</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" t="s" s="0">
         <v>53</v>
       </c>
@@ -4377,7 +4379,7 @@
         <v>308</v>
       </c>
       <c r="I50" t="s" s="0">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="K50" t="s" s="0">
         <v>264</v>
@@ -4395,10 +4397,10 @@
         <v>42490</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" t="s" s="0">
         <v>53</v>
       </c>
@@ -4424,13 +4426,13 @@
         <v>309</v>
       </c>
       <c r="I51" t="s" s="0">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="K51" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L51" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M51" s="0">
         <v>178</v>
@@ -4442,10 +4444,10 @@
         <v>39101</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s" s="0">
         <v>13</v>
       </c>
@@ -4471,7 +4473,7 @@
         <v>310</v>
       </c>
       <c r="I52" t="s" s="0">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="K52" t="s" s="0">
         <v>264</v>
@@ -4489,10 +4491,10 @@
         <v>44962</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s" s="0">
         <v>14</v>
       </c>
@@ -4518,7 +4520,7 @@
         <v>311</v>
       </c>
       <c r="I53" t="s" s="0">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="K53" t="s" s="0">
         <v>264</v>
@@ -4536,10 +4538,10 @@
         <v>42148</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s" s="0">
         <v>15</v>
       </c>
@@ -4565,13 +4567,13 @@
         <v>312</v>
       </c>
       <c r="I54" t="s" s="0">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="K54" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L54" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M54" s="0">
         <v>556</v>
@@ -4583,10 +4585,10 @@
         <v>43805</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s" s="0">
         <v>15</v>
       </c>
@@ -4612,7 +4614,7 @@
         <v>313</v>
       </c>
       <c r="I55" t="s" s="0">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K55" t="s" s="0">
         <v>264</v>
@@ -4630,34 +4632,34 @@
         <v>40575</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D56" s="1"/>
       <c r="E56" s="4"/>
       <c r="F56" s="6"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D57" s="1"/>
       <c r="E57" s="4"/>
       <c r="F57" s="6"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D58" s="1"/>
       <c r="E58" s="4"/>
       <c r="F58" s="6"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D59" s="1"/>
       <c r="E59" s="4"/>
       <c r="F59" s="6"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" t="s" s="0">
         <v>19</v>
       </c>
@@ -4683,7 +4685,7 @@
         <v>314</v>
       </c>
       <c r="I60" t="s" s="0">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="K60" t="s" s="0">
         <v>264</v>
@@ -4701,10 +4703,10 @@
         <v>38607</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" t="s" s="0">
         <v>54</v>
       </c>
@@ -4730,7 +4732,7 @@
         <v>315</v>
       </c>
       <c r="I61" t="s" s="0">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="K61" t="s" s="0">
         <v>264</v>
@@ -4748,10 +4750,10 @@
         <v>42083</v>
       </c>
       <c r="Q61" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" t="s" s="0">
         <v>21</v>
       </c>
@@ -4777,13 +4779,13 @@
         <v>316</v>
       </c>
       <c r="I62" t="s" s="0">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="K62" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L62" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M62" s="0">
         <v>446</v>
@@ -4795,10 +4797,10 @@
         <v>39105</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" t="s" s="0">
         <v>22</v>
       </c>
@@ -4824,7 +4826,7 @@
         <v>317</v>
       </c>
       <c r="I63" t="s" s="0">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="K63" t="s" s="0">
         <v>264</v>
@@ -4842,10 +4844,10 @@
         <v>41938</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" t="s" s="0">
         <v>23</v>
       </c>
@@ -4868,7 +4870,7 @@
         <v>318</v>
       </c>
       <c r="I64" t="s" s="0">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="K64" t="s" s="0">
         <v>264</v>
@@ -4886,10 +4888,10 @@
         <v>43691</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" t="s" s="0">
         <v>55</v>
       </c>
@@ -4912,7 +4914,7 @@
         <v>319</v>
       </c>
       <c r="I65" t="s" s="0">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="K65" t="s" s="0">
         <v>264</v>
@@ -4930,10 +4932,10 @@
         <v>42810</v>
       </c>
       <c r="Q65" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" t="s" s="0">
         <v>24</v>
       </c>
@@ -4956,7 +4958,7 @@
         <v>320</v>
       </c>
       <c r="I66" t="s" s="0">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="K66" t="s" s="0">
         <v>264</v>
@@ -4974,10 +4976,10 @@
         <v>45570</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" t="s" s="0">
         <v>25</v>
       </c>
@@ -5003,7 +5005,7 @@
         <v>321</v>
       </c>
       <c r="I67" t="s" s="0">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="K67" t="s" s="0">
         <v>264</v>
@@ -5021,10 +5023,10 @@
         <v>40799</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" t="s" s="0">
         <v>26</v>
       </c>
@@ -5050,7 +5052,7 @@
         <v>322</v>
       </c>
       <c r="I68" t="s" s="0">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="K68" t="s" s="0">
         <v>264</v>
@@ -5068,10 +5070,10 @@
         <v>42926</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" t="s" s="0">
         <v>27</v>
       </c>
@@ -5097,13 +5099,13 @@
         <v>323</v>
       </c>
       <c r="I69" t="s" s="0">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="K69" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L69" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M69" s="0">
         <v>983</v>
@@ -5115,10 +5117,10 @@
         <v>43569</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" t="s" s="0">
         <v>16</v>
       </c>
@@ -5144,7 +5146,7 @@
         <v>324</v>
       </c>
       <c r="I70" t="s" s="0">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="K70" t="s" s="0">
         <v>264</v>
@@ -5162,10 +5164,10 @@
         <v>42657</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" t="s" s="0">
         <v>17</v>
       </c>
@@ -5191,7 +5193,7 @@
         <v>314</v>
       </c>
       <c r="I71" t="s" s="0">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="K71" t="s" s="0">
         <v>264</v>
@@ -5209,10 +5211,10 @@
         <v>38841</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" t="s" s="0">
         <v>18</v>
       </c>
@@ -5238,7 +5240,7 @@
         <v>325</v>
       </c>
       <c r="I72" t="s" s="0">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="K72" t="s" s="0">
         <v>264</v>
@@ -5256,10 +5258,10 @@
         <v>42522</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" t="s" s="0">
         <v>18</v>
       </c>
@@ -5285,7 +5287,7 @@
         <v>326</v>
       </c>
       <c r="I73" t="s" s="0">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="K73" t="s" s="0">
         <v>264</v>
@@ -5303,10 +5305,10 @@
         <v>39748</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" t="s" s="0">
         <v>56</v>
       </c>
@@ -5332,13 +5334,13 @@
         <v>327</v>
       </c>
       <c r="I74" t="s" s="0">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="K74" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L74" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M74" s="0">
         <v>545</v>
@@ -5350,10 +5352,10 @@
         <v>40427</v>
       </c>
       <c r="Q74" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" t="s" s="0">
         <v>57</v>
       </c>
@@ -5379,7 +5381,7 @@
         <v>328</v>
       </c>
       <c r="I75" t="s" s="0">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="K75" t="s" s="0">
         <v>264</v>
@@ -5397,10 +5399,10 @@
         <v>42543</v>
       </c>
       <c r="Q75" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" t="s" s="0">
         <v>58</v>
       </c>
@@ -5426,7 +5428,7 @@
         <v>329</v>
       </c>
       <c r="I76" t="s" s="0">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="K76" t="s" s="0">
         <v>264</v>
@@ -5444,10 +5446,10 @@
         <v>45341</v>
       </c>
       <c r="Q76" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" t="s" s="0">
         <v>59</v>
       </c>
@@ -5470,10 +5472,10 @@
         <v>363</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="I77" t="s" s="0">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="K77" t="s" s="0">
         <v>264</v>
@@ -5491,16 +5493,16 @@
         <v>39295</v>
       </c>
       <c r="Q77" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D78" s="1"/>
       <c r="E78" s="4"/>
       <c r="F78" s="6"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s" s="0">
         <v>60</v>
       </c>
@@ -5526,7 +5528,7 @@
         <v>331</v>
       </c>
       <c r="I79" t="s" s="0">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="K79" t="s" s="0">
         <v>264</v>
@@ -5544,10 +5546,10 @@
         <v>38315</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" t="s" s="0">
         <v>61</v>
       </c>
@@ -5570,16 +5572,16 @@
         <v>363</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="I80" t="s" s="0">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="K80" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L80" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M80" s="0">
         <v>692</v>
@@ -5591,10 +5593,10 @@
         <v>43991</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" t="s" s="0">
         <v>62</v>
       </c>
@@ -5620,7 +5622,7 @@
         <v>333</v>
       </c>
       <c r="I81" t="s" s="0">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="K81" t="s" s="0">
         <v>264</v>
@@ -5638,10 +5640,10 @@
         <v>45030</v>
       </c>
       <c r="Q81" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" t="s" s="0">
         <v>63</v>
       </c>
@@ -5667,7 +5669,7 @@
         <v>334</v>
       </c>
       <c r="I82" t="s" s="0">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="K82" t="s" s="0">
         <v>264</v>
@@ -5685,10 +5687,10 @@
         <v>40558</v>
       </c>
       <c r="Q82" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" t="s" s="0">
         <v>64</v>
       </c>
@@ -5711,10 +5713,10 @@
         <v>376</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="I83" t="s" s="0">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="K83" t="s" s="0">
         <v>264</v>
@@ -5732,10 +5734,10 @@
         <v>42650</v>
       </c>
       <c r="Q83" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" t="s" s="0">
         <v>65</v>
       </c>
@@ -5758,7 +5760,7 @@
         <v>336</v>
       </c>
       <c r="I84" t="s" s="0">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="K84" t="s" s="0">
         <v>264</v>
@@ -5776,16 +5778,16 @@
         <v>41024</v>
       </c>
       <c r="Q84" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D85" s="1"/>
       <c r="E85" s="4"/>
       <c r="F85" s="6"/>
       <c r="H85" s="3"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" t="s" s="0">
         <v>66</v>
       </c>
@@ -5811,13 +5813,13 @@
         <v>337</v>
       </c>
       <c r="I86" t="s" s="0">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="K86" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L86" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M86" s="0">
         <v>597</v>
@@ -5829,10 +5831,10 @@
         <v>45627</v>
       </c>
       <c r="Q86" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" t="s" s="0">
         <v>67</v>
       </c>
@@ -5858,7 +5860,7 @@
         <v>338</v>
       </c>
       <c r="I87" t="s" s="0">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="K87" t="s" s="0">
         <v>264</v>
@@ -5876,10 +5878,10 @@
         <v>39308</v>
       </c>
       <c r="Q87" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" t="s" s="0">
         <v>68</v>
       </c>
@@ -5905,7 +5907,7 @@
         <v>339</v>
       </c>
       <c r="I88" t="s" s="0">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="K88" t="s" s="0">
         <v>264</v>
@@ -5923,10 +5925,10 @@
         <v>40028</v>
       </c>
       <c r="Q88" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" t="s" s="0">
         <v>69</v>
       </c>
@@ -5952,7 +5954,7 @@
         <v>340</v>
       </c>
       <c r="I89" t="s" s="0">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="K89" t="s" s="0">
         <v>264</v>
@@ -5970,10 +5972,10 @@
         <v>39734</v>
       </c>
       <c r="Q89" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" t="s" s="0">
         <v>52</v>
       </c>
@@ -5996,7 +5998,7 @@
         <v>341</v>
       </c>
       <c r="I90" t="s" s="0">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="K90" t="s" s="0">
         <v>264</v>
@@ -6014,10 +6016,10 @@
         <v>40418</v>
       </c>
       <c r="Q90" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" t="s" s="0">
         <v>70</v>
       </c>
@@ -6043,7 +6045,7 @@
         <v>342</v>
       </c>
       <c r="I91" t="s" s="0">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="K91" t="s" s="0">
         <v>264</v>
@@ -6061,10 +6063,10 @@
         <v>39480</v>
       </c>
       <c r="Q91" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" t="s" s="0">
         <v>71</v>
       </c>
@@ -6090,7 +6092,7 @@
         <v>343</v>
       </c>
       <c r="I92" t="s" s="0">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="K92" t="s" s="0">
         <v>264</v>
@@ -6108,10 +6110,10 @@
         <v>39939</v>
       </c>
       <c r="Q92" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" t="s" s="0">
         <v>72</v>
       </c>
@@ -6137,13 +6139,13 @@
         <v>344</v>
       </c>
       <c r="I93" t="s" s="0">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="K93" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L93" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M93" s="0">
         <v>76</v>
@@ -6155,10 +6157,10 @@
         <v>41007</v>
       </c>
       <c r="Q93" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" t="s" s="0">
         <v>73</v>
       </c>
@@ -6182,7 +6184,7 @@
         <v>345</v>
       </c>
       <c r="I94" t="s" s="0">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="K94" t="s" s="0">
         <v>264</v>
@@ -6200,10 +6202,10 @@
         <v>41247</v>
       </c>
       <c r="Q94" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" t="s" s="0">
         <v>74</v>
       </c>
@@ -6229,7 +6231,7 @@
         <v>346</v>
       </c>
       <c r="I95" t="s" s="0">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="K95" t="s" s="0">
         <v>264</v>
@@ -6247,46 +6249,46 @@
         <v>45099</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D96" s="1"/>
       <c r="E96" s="4"/>
       <c r="F96" s="6"/>
       <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D97" s="1"/>
       <c r="E97" s="4"/>
       <c r="F97" s="6"/>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D98" s="1"/>
       <c r="E98" s="4"/>
       <c r="F98" s="6"/>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D99" s="1"/>
       <c r="E99" s="4"/>
       <c r="F99" s="6"/>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D100" s="1"/>
       <c r="E100" s="4"/>
       <c r="F100" s="6"/>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D101" s="1"/>
       <c r="E101" s="4"/>
       <c r="F101" s="6"/>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" t="s" s="0">
         <v>56</v>
       </c>
@@ -6309,10 +6311,10 @@
         <v>373</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="I102" t="s" s="0">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="K102" t="s" s="0">
         <v>264</v>
@@ -6330,10 +6332,10 @@
         <v>40726</v>
       </c>
       <c r="Q102" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s" s="0">
         <v>57</v>
       </c>
@@ -6356,16 +6358,16 @@
         <v>374</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="I103" t="s" s="0">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="K103" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L103" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M103" s="0">
         <v>964</v>
@@ -6377,10 +6379,10 @@
         <v>44937</v>
       </c>
       <c r="Q103" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s" s="0">
         <v>58</v>
       </c>
@@ -6406,7 +6408,7 @@
         <v>349</v>
       </c>
       <c r="I104" t="s" s="0">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="K104" t="s" s="0">
         <v>264</v>
@@ -6424,10 +6426,10 @@
         <v>40195</v>
       </c>
       <c r="Q104" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" t="s" s="0">
         <v>59</v>
       </c>
@@ -6453,7 +6455,7 @@
         <v>350</v>
       </c>
       <c r="I105" t="s" s="0">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="K105" t="s" s="0">
         <v>264</v>
@@ -6471,10 +6473,10 @@
         <v>40974</v>
       </c>
       <c r="Q105" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s" s="0">
         <v>13</v>
       </c>
@@ -6497,16 +6499,16 @@
         <v>381</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="I106" t="s" s="0">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="K106" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L106" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M106" s="0">
         <v>188</v>
@@ -6518,130 +6520,130 @@
         <v>44615</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D107" s="1"/>
       <c r="E107" s="4"/>
       <c r="F107" s="6"/>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D108" s="1"/>
       <c r="E108" s="4"/>
       <c r="F108" s="6"/>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D109" s="1"/>
       <c r="E109" s="4"/>
       <c r="F109" s="6"/>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D110" s="1"/>
       <c r="E110" s="4"/>
       <c r="F110" s="6"/>
       <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D111" s="1"/>
       <c r="E111" s="4"/>
       <c r="F111" s="6"/>
       <c r="H111" s="3"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D112" s="1"/>
       <c r="E112" s="4"/>
       <c r="F112" s="6"/>
       <c r="H112" s="3"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D113" s="1"/>
       <c r="E113" s="4"/>
       <c r="F113" s="6"/>
       <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D114" s="1"/>
       <c r="E114" s="4"/>
       <c r="F114" s="6"/>
       <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D115" s="1"/>
       <c r="E115" s="4"/>
       <c r="F115" s="6"/>
       <c r="H115" s="3"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D116" s="1"/>
       <c r="E116" s="4"/>
       <c r="F116" s="6"/>
       <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D117" s="1"/>
       <c r="E117" s="4"/>
       <c r="F117" s="6"/>
       <c r="H117" s="3"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D118" s="1"/>
       <c r="E118" s="4"/>
       <c r="F118" s="6"/>
       <c r="H118" s="3"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D119" s="1"/>
       <c r="E119" s="4"/>
       <c r="F119" s="6"/>
       <c r="H119" s="3"/>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D120" s="1"/>
       <c r="E120" s="4"/>
       <c r="F120" s="6"/>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D121" s="1"/>
       <c r="E121" s="4"/>
       <c r="F121" s="6"/>
       <c r="H121" s="3"/>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D122" s="1"/>
       <c r="E122" s="4"/>
       <c r="F122" s="6"/>
       <c r="H122" s="3"/>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D123" s="1"/>
       <c r="E123" s="4"/>
       <c r="F123" s="6"/>
       <c r="H123" s="3"/>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D124" s="1"/>
       <c r="E124" s="4"/>
       <c r="F124" s="6"/>
       <c r="H124" s="3"/>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D125" s="1"/>
       <c r="E125" s="4"/>
       <c r="F125" s="6"/>
       <c r="H125" s="3"/>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D126" s="1"/>
       <c r="E126" s="4"/>
       <c r="F126" s="6"/>
       <c r="H126" s="3"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" t="s" s="0">
         <v>75</v>
       </c>
@@ -6667,7 +6669,7 @@
         <v>352</v>
       </c>
       <c r="I127" t="s" s="0">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="K127" t="s" s="0">
         <v>264</v>
@@ -6685,10 +6687,10 @@
         <v>39738</v>
       </c>
       <c r="Q127" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" t="s" s="0">
         <v>76</v>
       </c>
@@ -6711,10 +6713,10 @@
         <v>369</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I128" t="s" s="0">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="K128" t="s" s="0">
         <v>264</v>
@@ -6732,10 +6734,10 @@
         <v>40453</v>
       </c>
       <c r="Q128" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s" s="0">
         <v>77</v>
       </c>
@@ -6761,7 +6763,7 @@
         <v>354</v>
       </c>
       <c r="I129" t="s" s="0">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="K129" t="s" s="0">
         <v>264</v>
@@ -6779,10 +6781,10 @@
         <v>43473</v>
       </c>
       <c r="Q129" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s" s="0">
         <v>68</v>
       </c>
@@ -6808,13 +6810,13 @@
         <v>355</v>
       </c>
       <c r="I130" t="s" s="0">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="K130" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L130" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M130" s="0">
         <v>1</v>
@@ -6826,10 +6828,10 @@
         <v>40935</v>
       </c>
       <c r="Q130" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" t="s" s="0">
         <v>69</v>
       </c>
@@ -6855,7 +6857,7 @@
         <v>356</v>
       </c>
       <c r="I131" t="s" s="0">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="K131" t="s" s="0">
         <v>264</v>
@@ -6873,10 +6875,10 @@
         <v>44175</v>
       </c>
       <c r="Q131" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s" s="0">
         <v>52</v>
       </c>
@@ -6902,10 +6904,10 @@
         <v>357</v>
       </c>
       <c r="I132" t="s" s="0">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="K132" t="s" s="0">
-        <v>500</v>
+        <v>264</v>
       </c>
       <c r="L132" s="0">
         <v>0</v>
@@ -6920,10 +6922,10 @@
         <v>40887</v>
       </c>
       <c r="Q132" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" t="s" s="0">
         <v>70</v>
       </c>
@@ -6949,7 +6951,7 @@
         <v>358</v>
       </c>
       <c r="I133" t="s" s="0">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="K133" t="s" s="0">
         <v>264</v>
@@ -6967,10 +6969,10 @@
         <v>43334</v>
       </c>
       <c r="Q133" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s" s="0">
         <v>71</v>
       </c>
@@ -6996,13 +6998,13 @@
         <v>359</v>
       </c>
       <c r="I134" t="s" s="0">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="K134" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L134" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M134" s="0">
         <v>728</v>
@@ -7014,10 +7016,10 @@
         <v>42557</v>
       </c>
       <c r="Q134" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" t="s" s="0">
         <v>72</v>
       </c>
@@ -7041,7 +7043,7 @@
         <v>360</v>
       </c>
       <c r="I135" t="s" s="0">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="K135" t="s" s="0">
         <v>264</v>
@@ -7059,10 +7061,10 @@
         <v>43929</v>
       </c>
       <c r="Q135" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s" s="0">
         <v>73</v>
       </c>
@@ -7088,7 +7090,7 @@
         <v>361</v>
       </c>
       <c r="I136" t="s" s="0">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="K136" t="s" s="0">
         <v>264</v>
@@ -7106,69 +7108,69 @@
         <v>40457</v>
       </c>
       <c r="Q136" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E137" s="4"/>
       <c r="F137" s="6"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E138" s="4"/>
       <c r="F138" s="6"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E139" s="4"/>
       <c r="F139" s="6"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E140" s="4"/>
       <c r="F140" s="6"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E141" s="4"/>
       <c r="F141" s="6"/>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E142" s="4"/>
       <c r="F142" s="6"/>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E143" s="4"/>
       <c r="F143" s="6"/>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E144" s="4"/>
       <c r="F144" s="6"/>
     </row>
-    <row r="145" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E145" s="4"/>
       <c r="F145" s="6"/>
     </row>
-    <row r="146" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E146" s="4"/>
       <c r="F146" s="6"/>
     </row>
-    <row r="147" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E147" s="4"/>
       <c r="F147" s="6"/>
     </row>
-    <row r="148" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E148" s="4"/>
       <c r="F148" s="6"/>
     </row>
-    <row r="149" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E149" s="4"/>
       <c r="F149" s="6"/>
     </row>
-    <row r="150" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E150" s="4"/>
       <c r="F150" s="6"/>
     </row>
-    <row r="151" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:6" x14ac:dyDescent="0.3">
       <c r="F151" s="6"/>
     </row>
-    <row r="152" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="5:6" x14ac:dyDescent="0.3">
       <c r="F152" s="6"/>
     </row>
   </sheetData>
@@ -7179,80 +7181,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A8F51-8D2A-4E56-BAC3-F686CC936FAB}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.85546875"/>
-    <col min="2" max="2" customWidth="true" width="14.85546875"/>
+    <col min="1" max="1" customWidth="true" width="15.88671875"/>
+    <col min="2" max="2" customWidth="true" width="14.88671875"/>
     <col min="6" max="6" customWidth="true" width="46.0"/>
-    <col min="7" max="7" customWidth="true" width="14.28515625"/>
-    <col min="11" max="12" customWidth="true" width="20.7109375"/>
+    <col min="7" max="7" customWidth="true" width="14.33203125"/>
+    <col min="11" max="12" customWidth="true" width="20.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
         <v>470</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="C1" t="s" s="0">
         <v>469</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="G1" t="s" s="0">
         <v>467</v>
       </c>
       <c r="H1" t="s" s="0">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="I1" t="s" s="0">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="J1" t="s" s="0">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="K1" t="s" s="0">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="L1" t="s" s="0">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="M1" t="s" s="0">
         <v>468</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>501</v>
+        <v>471</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C2" s="0">
         <v>1</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>264</v>
@@ -7267,24 +7269,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
-        <v>501</v>
+        <v>471</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C3" s="0">
         <v>1</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>264</v>
@@ -7299,24 +7301,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
-        <v>501</v>
+        <v>471</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C4" s="0">
         <v>1</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>264</v>
@@ -7331,460 +7333,219 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
-        <v>501</v>
+        <v>471</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C5" s="0">
         <v>1</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>264</v>
       </c>
       <c r="I5" s="0">
-        <v>100</v>
+        <v>9999</v>
       </c>
       <c r="J5" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5" s="0">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
-        <v>501</v>
+        <v>471</v>
       </c>
       <c r="B6" t="s" s="0">
+        <v>472</v>
+      </c>
+      <c r="C6" s="0">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>489</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>481</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="H6" s="0">
+        <v>12</v>
+      </c>
+      <c r="I6" s="0">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s" s="0">
         <v>471</v>
       </c>
-      <c r="C6" s="0">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>479</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>502</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>503</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>264</v>
-      </c>
-      <c r="I6" s="0">
-        <v>9999</v>
-      </c>
-      <c r="J6" s="0">
-        <v>5</v>
-      </c>
-      <c r="M6" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s" s="0">
-        <v>501</v>
-      </c>
       <c r="B7" t="s" s="0">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C7" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>489</v>
+        <v>500</v>
       </c>
       <c r="K7" s="0">
         <v>10</v>
       </c>
       <c r="L7" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M7" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s" s="0">
-        <v>501</v>
+        <v>471</v>
       </c>
       <c r="B8" t="s" s="0">
+        <v>493</v>
+      </c>
+      <c r="C8" s="0">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>481</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>482</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="H8" s="0">
+        <v>50</v>
+      </c>
+      <c r="I8" s="0">
+        <v>20</v>
+      </c>
+      <c r="M8" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s" s="0">
         <v>471</v>
       </c>
-      <c r="C8" s="0">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>496</v>
-      </c>
-      <c r="K8" s="0">
-        <v>10</v>
-      </c>
-      <c r="L8" s="0">
-        <v>1</v>
-      </c>
-      <c r="M8" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s" s="0">
-        <v>501</v>
-      </c>
       <c r="B9" t="s" s="0">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="C9" s="0">
         <v>4</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>500</v>
-      </c>
-      <c r="H9" s="0">
-        <v>50</v>
+        <v>264</v>
       </c>
       <c r="I9" s="0">
-        <v>20</v>
+        <v>9999</v>
+      </c>
+      <c r="J9" s="0">
+        <v>0.75</v>
       </c>
       <c r="M9" s="0">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s" s="0">
-        <v>501</v>
+        <v>471</v>
       </c>
       <c r="B10" t="s" s="0">
+        <v>493</v>
+      </c>
+      <c r="C10" s="0">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>491</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>481</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="H10" s="0">
+        <v>25</v>
+      </c>
+      <c r="M10" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s" s="0">
+        <v>471</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>503</v>
+      </c>
+      <c r="C11" s="0">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>473</v>
+      </c>
+      <c r="F11" t="s" s="0">
         <v>504</v>
       </c>
-      <c r="C10" s="0">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>479</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>482</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>483</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>500</v>
-      </c>
-      <c r="I10" s="0">
-        <v>50</v>
-      </c>
-      <c r="J10" s="0">
-        <v>1</v>
-      </c>
-      <c r="M10" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s" s="0">
-        <v>501</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>504</v>
-      </c>
-      <c r="C11" s="0">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>479</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>484</v>
-      </c>
-      <c r="F11" t="s" s="0">
-        <v>485</v>
-      </c>
       <c r="G11" t="s" s="0">
-        <v>500</v>
+        <v>505</v>
+      </c>
+      <c r="H11" s="0">
+        <v>20</v>
       </c>
       <c r="I11" s="0">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J11" s="0">
         <v>2</v>
       </c>
       <c r="M11" s="0">
         <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s" s="0">
-        <v>501</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>504</v>
-      </c>
-      <c r="C12" s="0">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>479</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>486</v>
-      </c>
-      <c r="F12" t="s" s="0">
-        <v>487</v>
-      </c>
-      <c r="G12" t="s" s="0">
-        <v>500</v>
-      </c>
-      <c r="I12" s="0">
-        <v>100</v>
-      </c>
-      <c r="J12" s="0">
-        <v>5</v>
-      </c>
-      <c r="M12" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s" s="0">
-        <v>501</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>504</v>
-      </c>
-      <c r="C13" s="0">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>479</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>502</v>
-      </c>
-      <c r="F13" t="s" s="0">
-        <v>503</v>
-      </c>
-      <c r="G13" t="s" s="0">
-        <v>500</v>
-      </c>
-      <c r="I13" s="0">
-        <v>9999</v>
-      </c>
-      <c r="J13" s="0">
-        <v>10</v>
-      </c>
-      <c r="M13" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s" s="0">
-        <v>501</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>504</v>
-      </c>
-      <c r="C14" s="0">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="E14" t="s" s="0">
-        <v>480</v>
-      </c>
-      <c r="F14" t="s" s="0">
-        <v>489</v>
-      </c>
-      <c r="H14" s="0">
-        <v>25</v>
-      </c>
-      <c r="M14" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s" s="0">
-        <v>501</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>498</v>
-      </c>
-      <c r="C15" s="0">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s" s="0">
-        <v>479</v>
-      </c>
-      <c r="E15" t="s" s="0">
-        <v>472</v>
-      </c>
-      <c r="F15" t="s" s="0">
-        <v>499</v>
-      </c>
-      <c r="G15" t="s" s="0">
-        <v>500</v>
-      </c>
-      <c r="H15" s="0">
-        <v>20</v>
-      </c>
-      <c r="I15" s="0">
-        <v>30</v>
-      </c>
-      <c r="J15" s="0">
-        <v>2</v>
-      </c>
-      <c r="M15" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s" s="0">
-        <v>501</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>471</v>
-      </c>
-      <c r="C16" s="0">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="E16" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="F16" t="s" s="0">
-        <v>496</v>
-      </c>
-      <c r="K16" s="0">
-        <v>10</v>
-      </c>
-      <c r="L16" s="0">
-        <v>1</v>
-      </c>
-      <c r="M16" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s" s="0">
-        <v>501</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>498</v>
-      </c>
-      <c r="C17" s="0">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s" s="0">
-        <v>488</v>
-      </c>
-      <c r="E17" t="s" s="0">
-        <v>480</v>
-      </c>
-      <c r="F17" t="s" s="0">
-        <v>505</v>
-      </c>
-      <c r="H17" s="0">
-        <v>30</v>
-      </c>
-      <c r="M17" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s" s="0">
-        <v>501</v>
-      </c>
-      <c r="B18" t="s" s="0">
-        <v>498</v>
-      </c>
-      <c r="C18" s="0">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="E18" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="F18" t="s" s="0">
-        <v>496</v>
-      </c>
-      <c r="K18" s="0">
-        <v>20</v>
-      </c>
-      <c r="L18" s="0">
-        <v>9</v>
-      </c>
-      <c r="M18" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s" s="0">
-        <v>501</v>
-      </c>
-      <c r="B19" t="s" s="0">
-        <v>504</v>
-      </c>
-      <c r="C19" s="0">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s" s="0">
-        <v>488</v>
-      </c>
-      <c r="E19" t="s" s="0">
-        <v>480</v>
-      </c>
-      <c r="F19" t="s" s="0">
-        <v>506</v>
-      </c>
-      <c r="K19" s="0">
-        <v>10</v>
-      </c>
-      <c r="L19" s="0">
-        <v>4</v>
-      </c>
-      <c r="M19" s="0">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizado diseño del PDF. Falta implementación, datos, ruta y conexión a base de datos.
</commit_message>
<xml_diff>
--- a/resources/SistemasAgua.xlsx
+++ b/resources/SistemasAgua.xlsx
@@ -5,39 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hds_8\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\202898\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA42F524-A6D0-442B-A471-5D24016F1AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FF753A-F146-4478-9E33-87A6307BEA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FF8BD292-BC82-4648-93FB-5EF5760864FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Contribuyente" sheetId="1" r:id="rId1"/>
     <sheet name="Ordenanza" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="614">
   <si>
     <t>Nombre</t>
   </si>
@@ -1452,9 +1441,6 @@
     <t>Pueblo</t>
   </si>
   <si>
-    <t>Prueba</t>
-  </si>
-  <si>
     <t>Hogar</t>
   </si>
   <si>
@@ -1518,36 +1504,24 @@
     <t>SobreQueConcepto</t>
   </si>
   <si>
-    <t>Empresa</t>
-  </si>
-  <si>
     <t>conceptosACobrar</t>
   </si>
   <si>
     <t>1 2 3</t>
   </si>
   <si>
-    <t>1 2</t>
-  </si>
-  <si>
     <t>TipoCalculo</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Importe Desagüe</t>
   </si>
   <si>
     <t>Juan</t>
   </si>
   <si>
-    <t>3 1</t>
-  </si>
-  <si>
     <t>PYME</t>
   </si>
   <si>
@@ -1555,6 +1529,30 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Astorga</t>
+  </si>
+  <si>
+    <t>Cuarto tramo</t>
+  </si>
+  <si>
+    <t>Agua cuarto tramo</t>
+  </si>
+  <si>
+    <t>Gran empresa</t>
+  </si>
+  <si>
+    <t>Precio fijo alcantarillado</t>
+  </si>
+  <si>
+    <t>Importe alcantarillado</t>
+  </si>
+  <si>
+    <t>4 5 10</t>
+  </si>
+  <si>
+    <t>6 8 9</t>
   </si>
   <si>
     <t>DK7331645124473461205164</t>
@@ -1948,9 +1946,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1988,7 +1986,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2094,7 +2092,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2236,7 +2234,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2246,22 +2244,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6ACB8-7F34-425E-9257-91AD8B97F35F}">
   <dimension ref="A1:Q152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q60" sqref="Q60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="30.109375"/>
-    <col min="6" max="6" customWidth="true" style="5" width="30.109375"/>
-    <col min="8" max="8" customWidth="true" width="22.5546875"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.88671875"/>
+    <col min="5" max="5" customWidth="true" width="30.140625"/>
+    <col min="6" max="6" customWidth="true" style="5" width="30.140625"/>
+    <col min="8" max="8" customWidth="true" width="22.5703125"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.85546875"/>
     <col min="14" max="14" customWidth="true" width="14.0"/>
-    <col min="15" max="15" style="7" width="11.44140625"/>
-    <col min="17" max="17" style="1" width="11.44140625"/>
+    <col min="15" max="15" style="7" width="11.42578125"/>
+    <col min="17" max="17" style="1" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -2311,12 +2309,12 @@
         <v>266</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>95</v>
@@ -2340,10 +2338,10 @@
         <v>267</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>264</v>
+        <v>500</v>
       </c>
       <c r="L2" s="0">
         <v>0</v>
@@ -2358,10 +2356,10 @@
         <v>45294</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
         <v>14</v>
       </c>
@@ -2387,7 +2385,7 @@
         <v>268</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="K3" t="s" s="0">
         <v>264</v>
@@ -2405,10 +2403,10 @@
         <v>38267</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
         <v>15</v>
       </c>
@@ -2434,7 +2432,7 @@
         <v>269</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="K4" t="s" s="0">
         <v>264</v>
@@ -2452,10 +2450,10 @@
         <v>39682</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="0">
         <v>15</v>
       </c>
@@ -2481,13 +2479,13 @@
         <v>270</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="K5" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L5" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M5" s="0">
         <v>942</v>
@@ -2499,10 +2497,10 @@
         <v>38765</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s" s="0">
         <v>16</v>
       </c>
@@ -2528,7 +2526,7 @@
         <v>271</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="K6" t="s" s="0">
         <v>264</v>
@@ -2546,10 +2544,10 @@
         <v>38646</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s" s="0">
         <v>17</v>
       </c>
@@ -2575,7 +2573,7 @@
         <v>272</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="K7" t="s" s="0">
         <v>264</v>
@@ -2593,10 +2591,10 @@
         <v>41039</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s" s="0">
         <v>18</v>
       </c>
@@ -2622,13 +2620,13 @@
         <v>273</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="K8" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L8" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M8" s="0">
         <v>586</v>
@@ -2640,10 +2638,10 @@
         <v>43912</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s" s="0">
         <v>18</v>
       </c>
@@ -2669,7 +2667,7 @@
         <v>274</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="K9" t="s" s="0">
         <v>264</v>
@@ -2687,10 +2685,10 @@
         <v>41745</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s" s="0">
         <v>19</v>
       </c>
@@ -2716,7 +2714,7 @@
         <v>275</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="K10" t="s" s="0">
         <v>264</v>
@@ -2734,10 +2732,10 @@
         <v>44978</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s" s="0">
         <v>20</v>
       </c>
@@ -2763,13 +2761,13 @@
         <v>276</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="K11" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L11" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M11" s="0">
         <v>645</v>
@@ -2781,10 +2779,10 @@
         <v>39134</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s" s="0">
         <v>21</v>
       </c>
@@ -2810,7 +2808,7 @@
         <v>277</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="K12" t="s" s="0">
         <v>264</v>
@@ -2828,10 +2826,10 @@
         <v>44614</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s" s="0">
         <v>22</v>
       </c>
@@ -2857,7 +2855,7 @@
         <v>278</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="K13" t="s" s="0">
         <v>264</v>
@@ -2875,10 +2873,10 @@
         <v>41490</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s" s="0">
         <v>23</v>
       </c>
@@ -2904,13 +2902,13 @@
         <v>279</v>
       </c>
       <c r="I14" t="s" s="0">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="K14" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L14" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M14" s="0">
         <v>72</v>
@@ -2922,16 +2920,16 @@
         <v>41228</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s" s="0">
         <v>24</v>
       </c>
@@ -2957,7 +2955,7 @@
         <v>280</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="K16" t="s" s="0">
         <v>264</v>
@@ -2975,10 +2973,10 @@
         <v>40637</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s" s="0">
         <v>25</v>
       </c>
@@ -3004,7 +3002,7 @@
         <v>281</v>
       </c>
       <c r="I17" t="s" s="0">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="K17" t="s" s="0">
         <v>264</v>
@@ -3022,10 +3020,10 @@
         <v>45079</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s" s="0">
         <v>26</v>
       </c>
@@ -3036,7 +3034,7 @@
         <v>144</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>393</v>
@@ -3051,7 +3049,7 @@
         <v>282</v>
       </c>
       <c r="I18" t="s" s="0">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="K18" t="s" s="0">
         <v>264</v>
@@ -3069,10 +3067,10 @@
         <v>43017</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s" s="0">
         <v>27</v>
       </c>
@@ -3098,13 +3096,13 @@
         <v>283</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="K19" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L19" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M19" s="0">
         <v>968</v>
@@ -3116,10 +3114,10 @@
         <v>39371</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s" s="0">
         <v>28</v>
       </c>
@@ -3145,7 +3143,7 @@
         <v>284</v>
       </c>
       <c r="I20" t="s" s="0">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="K20" t="s" s="0">
         <v>264</v>
@@ -3163,10 +3161,10 @@
         <v>39934</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s" s="0">
         <v>29</v>
       </c>
@@ -3192,7 +3190,7 @@
         <v>279</v>
       </c>
       <c r="I21" t="s" s="0">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="K21" t="s" s="0">
         <v>264</v>
@@ -3210,10 +3208,10 @@
         <v>43868</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s" s="0">
         <v>30</v>
       </c>
@@ -3236,13 +3234,13 @@
         <v>285</v>
       </c>
       <c r="I22" t="s" s="0">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="K22" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L22" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M22" s="0">
         <v>25</v>
@@ -3254,10 +3252,10 @@
         <v>41262</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s" s="0">
         <v>31</v>
       </c>
@@ -3280,7 +3278,7 @@
         <v>286</v>
       </c>
       <c r="I23" t="s" s="0">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="K23" t="s" s="0">
         <v>264</v>
@@ -3298,10 +3296,10 @@
         <v>45279</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s" s="0">
         <v>32</v>
       </c>
@@ -3324,7 +3322,7 @@
         <v>287</v>
       </c>
       <c r="I24" t="s" s="0">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="K24" t="s" s="0">
         <v>264</v>
@@ -3342,10 +3340,10 @@
         <v>39982</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s" s="0">
         <v>33</v>
       </c>
@@ -3368,13 +3366,13 @@
         <v>288</v>
       </c>
       <c r="I25" t="s" s="0">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="K25" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L25" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M25" s="0">
         <v>799</v>
@@ -3386,16 +3384,16 @@
         <v>41034</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s" s="0">
         <v>34</v>
       </c>
@@ -3421,7 +3419,7 @@
         <v>289</v>
       </c>
       <c r="I27" t="s" s="0">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="K27" t="s" s="0">
         <v>264</v>
@@ -3439,10 +3437,10 @@
         <v>39525</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s" s="0">
         <v>35</v>
       </c>
@@ -3468,13 +3466,13 @@
         <v>290</v>
       </c>
       <c r="I28" t="s" s="0">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="K28" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L28" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M28" s="0">
         <v>410</v>
@@ -3486,10 +3484,10 @@
         <v>42667</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s" s="0">
         <v>36</v>
       </c>
@@ -3515,7 +3513,7 @@
         <v>291</v>
       </c>
       <c r="I29" t="s" s="0">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="K29" t="s" s="0">
         <v>264</v>
@@ -3533,10 +3531,10 @@
         <v>44639</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s" s="0">
         <v>37</v>
       </c>
@@ -3562,7 +3560,7 @@
         <v>292</v>
       </c>
       <c r="I30" t="s" s="0">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="K30" t="s" s="0">
         <v>264</v>
@@ -3580,10 +3578,10 @@
         <v>37937</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s" s="0">
         <v>38</v>
       </c>
@@ -3609,7 +3607,7 @@
         <v>293</v>
       </c>
       <c r="I31" t="s" s="0">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="K31" t="s" s="0">
         <v>264</v>
@@ -3627,10 +3625,10 @@
         <v>43242</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s" s="0">
         <v>39</v>
       </c>
@@ -3656,7 +3654,7 @@
         <v>294</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="K32" t="s" s="0">
         <v>264</v>
@@ -3674,28 +3672,28 @@
         <v>39555</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s" s="0">
         <v>40</v>
       </c>
@@ -3721,13 +3719,13 @@
         <v>295</v>
       </c>
       <c r="I36" t="s" s="0">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="K36" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L36" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M36" s="0">
         <v>413</v>
@@ -3739,10 +3737,10 @@
         <v>43230</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s" s="0">
         <v>41</v>
       </c>
@@ -3768,7 +3766,7 @@
         <v>296</v>
       </c>
       <c r="I37" t="s" s="0">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="K37" t="s" s="0">
         <v>264</v>
@@ -3786,10 +3784,10 @@
         <v>38841</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s" s="0">
         <v>42</v>
       </c>
@@ -3815,7 +3813,7 @@
         <v>297</v>
       </c>
       <c r="I38" t="s" s="0">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="K38" t="s" s="0">
         <v>264</v>
@@ -3833,10 +3831,10 @@
         <v>44389</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s" s="0">
         <v>43</v>
       </c>
@@ -3862,7 +3860,7 @@
         <v>298</v>
       </c>
       <c r="I39" t="s" s="0">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="K39" t="s" s="0">
         <v>264</v>
@@ -3880,10 +3878,10 @@
         <v>45242</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s" s="0">
         <v>44</v>
       </c>
@@ -3909,7 +3907,7 @@
         <v>299</v>
       </c>
       <c r="I40" t="s" s="0">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="K40" t="s" s="0">
         <v>264</v>
@@ -3927,10 +3925,10 @@
         <v>41309</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s" s="0">
         <v>45</v>
       </c>
@@ -3956,7 +3954,7 @@
         <v>300</v>
       </c>
       <c r="I41" t="s" s="0">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="K41" t="s" s="0">
         <v>264</v>
@@ -3974,10 +3972,10 @@
         <v>45142</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s" s="0">
         <v>46</v>
       </c>
@@ -4003,7 +4001,7 @@
         <v>301</v>
       </c>
       <c r="I42" t="s" s="0">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="K42" t="s" s="0">
         <v>264</v>
@@ -4021,10 +4019,10 @@
         <v>45048</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s" s="0">
         <v>47</v>
       </c>
@@ -4050,7 +4048,7 @@
         <v>302</v>
       </c>
       <c r="I43" t="s" s="0">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="K43" t="s" s="0">
         <v>264</v>
@@ -4068,10 +4066,10 @@
         <v>44479</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s" s="0">
         <v>39</v>
       </c>
@@ -4097,7 +4095,7 @@
         <v>303</v>
       </c>
       <c r="I44" t="s" s="0">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="K44" t="s" s="0">
         <v>264</v>
@@ -4115,10 +4113,10 @@
         <v>42624</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s" s="0">
         <v>48</v>
       </c>
@@ -4144,7 +4142,7 @@
         <v>304</v>
       </c>
       <c r="I45" t="s" s="0">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="K45" t="s" s="0">
         <v>264</v>
@@ -4162,10 +4160,10 @@
         <v>42708</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s" s="0">
         <v>49</v>
       </c>
@@ -4191,7 +4189,7 @@
         <v>305</v>
       </c>
       <c r="I46" t="s" s="0">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="K46" t="s" s="0">
         <v>264</v>
@@ -4209,10 +4207,10 @@
         <v>44180</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s" s="0">
         <v>50</v>
       </c>
@@ -4238,7 +4236,7 @@
         <v>306</v>
       </c>
       <c r="I47" t="s" s="0">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="K47" t="s" s="0">
         <v>264</v>
@@ -4256,10 +4254,10 @@
         <v>45047</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s" s="0">
         <v>51</v>
       </c>
@@ -4285,13 +4283,13 @@
         <v>286</v>
       </c>
       <c r="I48" t="s" s="0">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="K48" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L48" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M48" s="0">
         <v>330</v>
@@ -4303,10 +4301,10 @@
         <v>42182</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s" s="0">
         <v>52</v>
       </c>
@@ -4332,7 +4330,7 @@
         <v>307</v>
       </c>
       <c r="I49" t="s" s="0">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="K49" t="s" s="0">
         <v>264</v>
@@ -4350,10 +4348,10 @@
         <v>43032</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s" s="0">
         <v>53</v>
       </c>
@@ -4379,7 +4377,7 @@
         <v>308</v>
       </c>
       <c r="I50" t="s" s="0">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="K50" t="s" s="0">
         <v>264</v>
@@ -4397,10 +4395,10 @@
         <v>42490</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s" s="0">
         <v>53</v>
       </c>
@@ -4426,13 +4424,13 @@
         <v>309</v>
       </c>
       <c r="I51" t="s" s="0">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="K51" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L51" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M51" s="0">
         <v>178</v>
@@ -4444,10 +4442,10 @@
         <v>39101</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s" s="0">
         <v>13</v>
       </c>
@@ -4473,7 +4471,7 @@
         <v>310</v>
       </c>
       <c r="I52" t="s" s="0">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="K52" t="s" s="0">
         <v>264</v>
@@ -4491,10 +4489,10 @@
         <v>44962</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s" s="0">
         <v>14</v>
       </c>
@@ -4520,7 +4518,7 @@
         <v>311</v>
       </c>
       <c r="I53" t="s" s="0">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="K53" t="s" s="0">
         <v>264</v>
@@ -4538,10 +4536,10 @@
         <v>42148</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s" s="0">
         <v>15</v>
       </c>
@@ -4567,13 +4565,13 @@
         <v>312</v>
       </c>
       <c r="I54" t="s" s="0">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="K54" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L54" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M54" s="0">
         <v>556</v>
@@ -4585,10 +4583,10 @@
         <v>43805</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s" s="0">
         <v>15</v>
       </c>
@@ -4614,7 +4612,7 @@
         <v>313</v>
       </c>
       <c r="I55" t="s" s="0">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="K55" t="s" s="0">
         <v>264</v>
@@ -4632,34 +4630,34 @@
         <v>40575</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="E56" s="4"/>
       <c r="F56" s="6"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="E57" s="4"/>
       <c r="F57" s="6"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="E58" s="4"/>
       <c r="F58" s="6"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="E59" s="4"/>
       <c r="F59" s="6"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s" s="0">
         <v>19</v>
       </c>
@@ -4685,7 +4683,7 @@
         <v>314</v>
       </c>
       <c r="I60" t="s" s="0">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="K60" t="s" s="0">
         <v>264</v>
@@ -4703,10 +4701,10 @@
         <v>38607</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s" s="0">
         <v>54</v>
       </c>
@@ -4732,7 +4730,7 @@
         <v>315</v>
       </c>
       <c r="I61" t="s" s="0">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="K61" t="s" s="0">
         <v>264</v>
@@ -4750,10 +4748,10 @@
         <v>42083</v>
       </c>
       <c r="Q61" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s" s="0">
         <v>21</v>
       </c>
@@ -4779,13 +4777,13 @@
         <v>316</v>
       </c>
       <c r="I62" t="s" s="0">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="K62" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L62" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M62" s="0">
         <v>446</v>
@@ -4797,10 +4795,10 @@
         <v>39105</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s" s="0">
         <v>22</v>
       </c>
@@ -4826,7 +4824,7 @@
         <v>317</v>
       </c>
       <c r="I63" t="s" s="0">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="K63" t="s" s="0">
         <v>264</v>
@@ -4844,10 +4842,10 @@
         <v>41938</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s" s="0">
         <v>23</v>
       </c>
@@ -4870,7 +4868,7 @@
         <v>318</v>
       </c>
       <c r="I64" t="s" s="0">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="K64" t="s" s="0">
         <v>264</v>
@@ -4888,10 +4886,10 @@
         <v>43691</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s" s="0">
         <v>55</v>
       </c>
@@ -4914,7 +4912,7 @@
         <v>319</v>
       </c>
       <c r="I65" t="s" s="0">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="K65" t="s" s="0">
         <v>264</v>
@@ -4932,10 +4930,10 @@
         <v>42810</v>
       </c>
       <c r="Q65" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s" s="0">
         <v>24</v>
       </c>
@@ -4958,7 +4956,7 @@
         <v>320</v>
       </c>
       <c r="I66" t="s" s="0">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="K66" t="s" s="0">
         <v>264</v>
@@ -4976,10 +4974,10 @@
         <v>45570</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s" s="0">
         <v>25</v>
       </c>
@@ -5005,7 +5003,7 @@
         <v>321</v>
       </c>
       <c r="I67" t="s" s="0">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="K67" t="s" s="0">
         <v>264</v>
@@ -5023,10 +5021,10 @@
         <v>40799</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s" s="0">
         <v>26</v>
       </c>
@@ -5052,7 +5050,7 @@
         <v>322</v>
       </c>
       <c r="I68" t="s" s="0">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="K68" t="s" s="0">
         <v>264</v>
@@ -5070,10 +5068,10 @@
         <v>42926</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s" s="0">
         <v>27</v>
       </c>
@@ -5099,13 +5097,13 @@
         <v>323</v>
       </c>
       <c r="I69" t="s" s="0">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="K69" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L69" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M69" s="0">
         <v>983</v>
@@ -5117,10 +5115,10 @@
         <v>43569</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s" s="0">
         <v>16</v>
       </c>
@@ -5146,7 +5144,7 @@
         <v>324</v>
       </c>
       <c r="I70" t="s" s="0">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="K70" t="s" s="0">
         <v>264</v>
@@ -5164,10 +5162,10 @@
         <v>42657</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s" s="0">
         <v>17</v>
       </c>
@@ -5193,7 +5191,7 @@
         <v>314</v>
       </c>
       <c r="I71" t="s" s="0">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="K71" t="s" s="0">
         <v>264</v>
@@ -5211,10 +5209,10 @@
         <v>38841</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s" s="0">
         <v>18</v>
       </c>
@@ -5240,7 +5238,7 @@
         <v>325</v>
       </c>
       <c r="I72" t="s" s="0">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="K72" t="s" s="0">
         <v>264</v>
@@ -5258,10 +5256,10 @@
         <v>42522</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s" s="0">
         <v>18</v>
       </c>
@@ -5287,7 +5285,7 @@
         <v>326</v>
       </c>
       <c r="I73" t="s" s="0">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="K73" t="s" s="0">
         <v>264</v>
@@ -5305,10 +5303,10 @@
         <v>39748</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s" s="0">
         <v>56</v>
       </c>
@@ -5334,13 +5332,13 @@
         <v>327</v>
       </c>
       <c r="I74" t="s" s="0">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="K74" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L74" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M74" s="0">
         <v>545</v>
@@ -5352,10 +5350,10 @@
         <v>40427</v>
       </c>
       <c r="Q74" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s" s="0">
         <v>57</v>
       </c>
@@ -5381,7 +5379,7 @@
         <v>328</v>
       </c>
       <c r="I75" t="s" s="0">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="K75" t="s" s="0">
         <v>264</v>
@@ -5399,10 +5397,10 @@
         <v>42543</v>
       </c>
       <c r="Q75" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s" s="0">
         <v>58</v>
       </c>
@@ -5428,7 +5426,7 @@
         <v>329</v>
       </c>
       <c r="I76" t="s" s="0">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="K76" t="s" s="0">
         <v>264</v>
@@ -5446,10 +5444,10 @@
         <v>45341</v>
       </c>
       <c r="Q76" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s" s="0">
         <v>59</v>
       </c>
@@ -5472,10 +5470,10 @@
         <v>363</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="I77" t="s" s="0">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="K77" t="s" s="0">
         <v>264</v>
@@ -5493,16 +5491,16 @@
         <v>39295</v>
       </c>
       <c r="Q77" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D78" s="1"/>
       <c r="E78" s="4"/>
       <c r="F78" s="6"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s" s="0">
         <v>60</v>
       </c>
@@ -5528,7 +5526,7 @@
         <v>331</v>
       </c>
       <c r="I79" t="s" s="0">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="K79" t="s" s="0">
         <v>264</v>
@@ -5546,10 +5544,10 @@
         <v>38315</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s" s="0">
         <v>61</v>
       </c>
@@ -5572,16 +5570,16 @@
         <v>363</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="I80" t="s" s="0">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="K80" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L80" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M80" s="0">
         <v>692</v>
@@ -5593,10 +5591,10 @@
         <v>43991</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s" s="0">
         <v>62</v>
       </c>
@@ -5622,7 +5620,7 @@
         <v>333</v>
       </c>
       <c r="I81" t="s" s="0">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="K81" t="s" s="0">
         <v>264</v>
@@ -5640,10 +5638,10 @@
         <v>45030</v>
       </c>
       <c r="Q81" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s" s="0">
         <v>63</v>
       </c>
@@ -5669,7 +5667,7 @@
         <v>334</v>
       </c>
       <c r="I82" t="s" s="0">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="K82" t="s" s="0">
         <v>264</v>
@@ -5687,10 +5685,10 @@
         <v>40558</v>
       </c>
       <c r="Q82" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s" s="0">
         <v>64</v>
       </c>
@@ -5713,10 +5711,10 @@
         <v>376</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="I83" t="s" s="0">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="K83" t="s" s="0">
         <v>264</v>
@@ -5734,10 +5732,10 @@
         <v>42650</v>
       </c>
       <c r="Q83" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s" s="0">
         <v>65</v>
       </c>
@@ -5760,7 +5758,7 @@
         <v>336</v>
       </c>
       <c r="I84" t="s" s="0">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="K84" t="s" s="0">
         <v>264</v>
@@ -5778,16 +5776,16 @@
         <v>41024</v>
       </c>
       <c r="Q84" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D85" s="1"/>
       <c r="E85" s="4"/>
       <c r="F85" s="6"/>
       <c r="H85" s="3"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s" s="0">
         <v>66</v>
       </c>
@@ -5813,13 +5811,13 @@
         <v>337</v>
       </c>
       <c r="I86" t="s" s="0">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="K86" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L86" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M86" s="0">
         <v>597</v>
@@ -5831,10 +5829,10 @@
         <v>45627</v>
       </c>
       <c r="Q86" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s" s="0">
         <v>67</v>
       </c>
@@ -5860,7 +5858,7 @@
         <v>338</v>
       </c>
       <c r="I87" t="s" s="0">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="K87" t="s" s="0">
         <v>264</v>
@@ -5878,10 +5876,10 @@
         <v>39308</v>
       </c>
       <c r="Q87" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s" s="0">
         <v>68</v>
       </c>
@@ -5907,7 +5905,7 @@
         <v>339</v>
       </c>
       <c r="I88" t="s" s="0">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="K88" t="s" s="0">
         <v>264</v>
@@ -5925,10 +5923,10 @@
         <v>40028</v>
       </c>
       <c r="Q88" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s" s="0">
         <v>69</v>
       </c>
@@ -5954,7 +5952,7 @@
         <v>340</v>
       </c>
       <c r="I89" t="s" s="0">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="K89" t="s" s="0">
         <v>264</v>
@@ -5972,10 +5970,10 @@
         <v>39734</v>
       </c>
       <c r="Q89" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s" s="0">
         <v>52</v>
       </c>
@@ -5998,7 +5996,7 @@
         <v>341</v>
       </c>
       <c r="I90" t="s" s="0">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="K90" t="s" s="0">
         <v>264</v>
@@ -6016,10 +6014,10 @@
         <v>40418</v>
       </c>
       <c r="Q90" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s" s="0">
         <v>70</v>
       </c>
@@ -6045,7 +6043,7 @@
         <v>342</v>
       </c>
       <c r="I91" t="s" s="0">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="K91" t="s" s="0">
         <v>264</v>
@@ -6063,10 +6061,10 @@
         <v>39480</v>
       </c>
       <c r="Q91" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s" s="0">
         <v>71</v>
       </c>
@@ -6092,7 +6090,7 @@
         <v>343</v>
       </c>
       <c r="I92" t="s" s="0">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="K92" t="s" s="0">
         <v>264</v>
@@ -6110,10 +6108,10 @@
         <v>39939</v>
       </c>
       <c r="Q92" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" t="s" s="0">
         <v>72</v>
       </c>
@@ -6139,13 +6137,13 @@
         <v>344</v>
       </c>
       <c r="I93" t="s" s="0">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K93" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L93" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M93" s="0">
         <v>76</v>
@@ -6157,10 +6155,10 @@
         <v>41007</v>
       </c>
       <c r="Q93" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s" s="0">
         <v>73</v>
       </c>
@@ -6184,7 +6182,7 @@
         <v>345</v>
       </c>
       <c r="I94" t="s" s="0">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="K94" t="s" s="0">
         <v>264</v>
@@ -6202,10 +6200,10 @@
         <v>41247</v>
       </c>
       <c r="Q94" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s" s="0">
         <v>74</v>
       </c>
@@ -6231,7 +6229,7 @@
         <v>346</v>
       </c>
       <c r="I95" t="s" s="0">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="K95" t="s" s="0">
         <v>264</v>
@@ -6249,46 +6247,46 @@
         <v>45099</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D96" s="1"/>
       <c r="E96" s="4"/>
       <c r="F96" s="6"/>
       <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D97" s="1"/>
       <c r="E97" s="4"/>
       <c r="F97" s="6"/>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D98" s="1"/>
       <c r="E98" s="4"/>
       <c r="F98" s="6"/>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D99" s="1"/>
       <c r="E99" s="4"/>
       <c r="F99" s="6"/>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D100" s="1"/>
       <c r="E100" s="4"/>
       <c r="F100" s="6"/>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D101" s="1"/>
       <c r="E101" s="4"/>
       <c r="F101" s="6"/>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s" s="0">
         <v>56</v>
       </c>
@@ -6311,10 +6309,10 @@
         <v>373</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="I102" t="s" s="0">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="K102" t="s" s="0">
         <v>264</v>
@@ -6332,10 +6330,10 @@
         <v>40726</v>
       </c>
       <c r="Q102" s="1" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s" s="0">
         <v>57</v>
       </c>
@@ -6358,16 +6356,16 @@
         <v>374</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="I103" t="s" s="0">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="K103" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L103" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M103" s="0">
         <v>964</v>
@@ -6379,10 +6377,10 @@
         <v>44937</v>
       </c>
       <c r="Q103" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s" s="0">
         <v>58</v>
       </c>
@@ -6408,7 +6406,7 @@
         <v>349</v>
       </c>
       <c r="I104" t="s" s="0">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="K104" t="s" s="0">
         <v>264</v>
@@ -6426,10 +6424,10 @@
         <v>40195</v>
       </c>
       <c r="Q104" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s" s="0">
         <v>59</v>
       </c>
@@ -6455,7 +6453,7 @@
         <v>350</v>
       </c>
       <c r="I105" t="s" s="0">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="K105" t="s" s="0">
         <v>264</v>
@@ -6473,10 +6471,10 @@
         <v>40974</v>
       </c>
       <c r="Q105" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s" s="0">
         <v>13</v>
       </c>
@@ -6499,16 +6497,16 @@
         <v>381</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="I106" t="s" s="0">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="K106" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L106" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M106" s="0">
         <v>188</v>
@@ -6520,130 +6518,130 @@
         <v>44615</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D107" s="1"/>
       <c r="E107" s="4"/>
       <c r="F107" s="6"/>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D108" s="1"/>
       <c r="E108" s="4"/>
       <c r="F108" s="6"/>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D109" s="1"/>
       <c r="E109" s="4"/>
       <c r="F109" s="6"/>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D110" s="1"/>
       <c r="E110" s="4"/>
       <c r="F110" s="6"/>
       <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D111" s="1"/>
       <c r="E111" s="4"/>
       <c r="F111" s="6"/>
       <c r="H111" s="3"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D112" s="1"/>
       <c r="E112" s="4"/>
       <c r="F112" s="6"/>
       <c r="H112" s="3"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D113" s="1"/>
       <c r="E113" s="4"/>
       <c r="F113" s="6"/>
       <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D114" s="1"/>
       <c r="E114" s="4"/>
       <c r="F114" s="6"/>
       <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D115" s="1"/>
       <c r="E115" s="4"/>
       <c r="F115" s="6"/>
       <c r="H115" s="3"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D116" s="1"/>
       <c r="E116" s="4"/>
       <c r="F116" s="6"/>
       <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D117" s="1"/>
       <c r="E117" s="4"/>
       <c r="F117" s="6"/>
       <c r="H117" s="3"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D118" s="1"/>
       <c r="E118" s="4"/>
       <c r="F118" s="6"/>
       <c r="H118" s="3"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D119" s="1"/>
       <c r="E119" s="4"/>
       <c r="F119" s="6"/>
       <c r="H119" s="3"/>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D120" s="1"/>
       <c r="E120" s="4"/>
       <c r="F120" s="6"/>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D121" s="1"/>
       <c r="E121" s="4"/>
       <c r="F121" s="6"/>
       <c r="H121" s="3"/>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D122" s="1"/>
       <c r="E122" s="4"/>
       <c r="F122" s="6"/>
       <c r="H122" s="3"/>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D123" s="1"/>
       <c r="E123" s="4"/>
       <c r="F123" s="6"/>
       <c r="H123" s="3"/>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D124" s="1"/>
       <c r="E124" s="4"/>
       <c r="F124" s="6"/>
       <c r="H124" s="3"/>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D125" s="1"/>
       <c r="E125" s="4"/>
       <c r="F125" s="6"/>
       <c r="H125" s="3"/>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D126" s="1"/>
       <c r="E126" s="4"/>
       <c r="F126" s="6"/>
       <c r="H126" s="3"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" t="s" s="0">
         <v>75</v>
       </c>
@@ -6669,7 +6667,7 @@
         <v>352</v>
       </c>
       <c r="I127" t="s" s="0">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="K127" t="s" s="0">
         <v>264</v>
@@ -6687,10 +6685,10 @@
         <v>39738</v>
       </c>
       <c r="Q127" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" t="s" s="0">
         <v>76</v>
       </c>
@@ -6713,10 +6711,10 @@
         <v>369</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="I128" t="s" s="0">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="K128" t="s" s="0">
         <v>264</v>
@@ -6734,10 +6732,10 @@
         <v>40453</v>
       </c>
       <c r="Q128" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s" s="0">
         <v>77</v>
       </c>
@@ -6763,7 +6761,7 @@
         <v>354</v>
       </c>
       <c r="I129" t="s" s="0">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="K129" t="s" s="0">
         <v>264</v>
@@ -6781,10 +6779,10 @@
         <v>43473</v>
       </c>
       <c r="Q129" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s" s="0">
         <v>68</v>
       </c>
@@ -6810,13 +6808,13 @@
         <v>355</v>
       </c>
       <c r="I130" t="s" s="0">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="K130" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L130" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M130" s="0">
         <v>1</v>
@@ -6828,10 +6826,10 @@
         <v>40935</v>
       </c>
       <c r="Q130" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" t="s" s="0">
         <v>69</v>
       </c>
@@ -6857,7 +6855,7 @@
         <v>356</v>
       </c>
       <c r="I131" t="s" s="0">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="K131" t="s" s="0">
         <v>264</v>
@@ -6875,10 +6873,10 @@
         <v>44175</v>
       </c>
       <c r="Q131" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" t="s" s="0">
         <v>52</v>
       </c>
@@ -6904,10 +6902,10 @@
         <v>357</v>
       </c>
       <c r="I132" t="s" s="0">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="K132" t="s" s="0">
-        <v>264</v>
+        <v>500</v>
       </c>
       <c r="L132" s="0">
         <v>0</v>
@@ -6922,10 +6920,10 @@
         <v>40887</v>
       </c>
       <c r="Q132" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" t="s" s="0">
         <v>70</v>
       </c>
@@ -6951,7 +6949,7 @@
         <v>358</v>
       </c>
       <c r="I133" t="s" s="0">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="K133" t="s" s="0">
         <v>264</v>
@@ -6969,10 +6967,10 @@
         <v>43334</v>
       </c>
       <c r="Q133" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" t="s" s="0">
         <v>71</v>
       </c>
@@ -6998,13 +6996,13 @@
         <v>359</v>
       </c>
       <c r="I134" t="s" s="0">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="K134" t="s" s="0">
         <v>264</v>
       </c>
       <c r="L134" s="0">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M134" s="0">
         <v>728</v>
@@ -7016,10 +7014,10 @@
         <v>42557</v>
       </c>
       <c r="Q134" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" t="s" s="0">
         <v>72</v>
       </c>
@@ -7043,7 +7041,7 @@
         <v>360</v>
       </c>
       <c r="I135" t="s" s="0">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="K135" t="s" s="0">
         <v>264</v>
@@ -7061,10 +7059,10 @@
         <v>43929</v>
       </c>
       <c r="Q135" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" t="s" s="0">
         <v>73</v>
       </c>
@@ -7090,7 +7088,7 @@
         <v>361</v>
       </c>
       <c r="I136" t="s" s="0">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="K136" t="s" s="0">
         <v>264</v>
@@ -7108,69 +7106,69 @@
         <v>40457</v>
       </c>
       <c r="Q136" s="1" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E137" s="4"/>
       <c r="F137" s="6"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E138" s="4"/>
       <c r="F138" s="6"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E139" s="4"/>
       <c r="F139" s="6"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E140" s="4"/>
       <c r="F140" s="6"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E141" s="4"/>
       <c r="F141" s="6"/>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E142" s="4"/>
       <c r="F142" s="6"/>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E143" s="4"/>
       <c r="F143" s="6"/>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E144" s="4"/>
       <c r="F144" s="6"/>
     </row>
-    <row r="145" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E145" s="4"/>
       <c r="F145" s="6"/>
     </row>
-    <row r="146" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E146" s="4"/>
       <c r="F146" s="6"/>
     </row>
-    <row r="147" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E147" s="4"/>
       <c r="F147" s="6"/>
     </row>
-    <row r="148" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E148" s="4"/>
       <c r="F148" s="6"/>
     </row>
-    <row r="149" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E149" s="4"/>
       <c r="F149" s="6"/>
     </row>
-    <row r="150" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E150" s="4"/>
       <c r="F150" s="6"/>
     </row>
-    <row r="151" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F151" s="6"/>
     </row>
-    <row r="152" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F152" s="6"/>
     </row>
   </sheetData>
@@ -7181,80 +7179,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A8F51-8D2A-4E56-BAC3-F686CC936FAB}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.88671875"/>
-    <col min="2" max="2" customWidth="true" width="14.88671875"/>
+    <col min="1" max="1" customWidth="true" width="15.85546875"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875"/>
     <col min="6" max="6" customWidth="true" width="46.0"/>
-    <col min="7" max="7" customWidth="true" width="14.33203125"/>
-    <col min="11" max="12" customWidth="true" width="20.6640625"/>
+    <col min="7" max="7" customWidth="true" width="14.28515625"/>
+    <col min="11" max="12" customWidth="true" width="20.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="0">
         <v>470</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C1" t="s" s="0">
         <v>469</v>
       </c>
       <c r="D1" t="s" s="0">
+        <v>472</v>
+      </c>
+      <c r="E1" t="s" s="0">
         <v>473</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="F1" t="s" s="0">
         <v>474</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>475</v>
       </c>
       <c r="G1" t="s" s="0">
         <v>467</v>
       </c>
       <c r="H1" t="s" s="0">
+        <v>475</v>
+      </c>
+      <c r="I1" t="s" s="0">
         <v>476</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="J1" t="s" s="0">
         <v>477</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="K1" t="s" s="0">
         <v>478</v>
       </c>
-      <c r="K1" t="s" s="0">
-        <v>479</v>
-      </c>
       <c r="L1" t="s" s="0">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="M1" t="s" s="0">
         <v>468</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>471</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>472</v>
       </c>
       <c r="C2" s="0">
         <v>1</v>
       </c>
       <c r="D2" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>480</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="F2" t="s" s="0">
         <v>481</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>482</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>264</v>
@@ -7269,24 +7267,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>471</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>472</v>
       </c>
       <c r="C3" s="0">
         <v>1</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E3" t="s" s="0">
+        <v>482</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>483</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>484</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>264</v>
@@ -7301,24 +7299,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>471</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>472</v>
       </c>
       <c r="C4" s="0">
         <v>1</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E4" t="s" s="0">
+        <v>484</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>485</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>486</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>264</v>
@@ -7333,219 +7331,460 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>471</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>472</v>
       </c>
       <c r="C5" s="0">
         <v>1</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E5" t="s" s="0">
+        <v>486</v>
+      </c>
+      <c r="F5" t="s" s="0">
         <v>487</v>
       </c>
-      <c r="F5" t="s" s="0">
-        <v>488</v>
-      </c>
       <c r="G5" t="s" s="0">
         <v>264</v>
       </c>
       <c r="I5" s="0">
-        <v>9999</v>
+        <v>100</v>
       </c>
       <c r="J5" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5" s="0">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>471</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>472</v>
-      </c>
       <c r="C6" s="0">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>502</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>503</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="I6" s="0">
+        <v>9999</v>
+      </c>
+      <c r="J6" s="0">
+        <v>5</v>
+      </c>
+      <c r="M6" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>471</v>
+      </c>
+      <c r="C7" s="0">
         <v>2</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D7" t="s" s="0">
+        <v>488</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="F7" t="s" s="0">
         <v>489</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>481</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="H6" s="0">
-        <v>12</v>
-      </c>
-      <c r="I6" s="0">
-        <v>0</v>
-      </c>
-      <c r="M6" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
-        <v>471</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>472</v>
-      </c>
-      <c r="C7" s="0">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>491</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>491</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>500</v>
       </c>
       <c r="K7" s="0">
         <v>10</v>
       </c>
       <c r="L7" s="0">
+        <v>3</v>
+      </c>
+      <c r="M7" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>471</v>
+      </c>
+      <c r="C8" s="0">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>496</v>
+      </c>
+      <c r="K8" s="0">
+        <v>10</v>
+      </c>
+      <c r="L8" s="0">
         <v>1</v>
       </c>
-      <c r="M7" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
-        <v>471</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>493</v>
-      </c>
-      <c r="C8" s="0">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>480</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>481</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>482</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>264</v>
-      </c>
-      <c r="H8" s="0">
-        <v>50</v>
-      </c>
-      <c r="I8" s="0">
-        <v>20</v>
-      </c>
       <c r="M8" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s" s="0">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="C9" s="0">
         <v>4</v>
       </c>
       <c r="D9" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E9" t="s" s="0">
         <v>480</v>
       </c>
-      <c r="E9" t="s" s="0">
-        <v>483</v>
-      </c>
       <c r="F9" t="s" s="0">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>264</v>
+        <v>500</v>
+      </c>
+      <c r="H9" s="0">
+        <v>50</v>
       </c>
       <c r="I9" s="0">
-        <v>9999</v>
-      </c>
-      <c r="J9" s="0">
-        <v>0.75</v>
+        <v>20</v>
       </c>
       <c r="M9" s="0">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s" s="0">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="C10" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>490</v>
-      </c>
-      <c r="H10" s="0">
-        <v>25</v>
+        <v>483</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>500</v>
+      </c>
+      <c r="I10" s="0">
+        <v>50</v>
+      </c>
+      <c r="J10" s="0">
+        <v>1</v>
       </c>
       <c r="M10" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s" s="0">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C11" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>473</v>
+        <v>484</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>504</v>
+        <v>485</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>505</v>
-      </c>
-      <c r="H11" s="0">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="I11" s="0">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J11" s="0">
         <v>2</v>
       </c>
       <c r="M11" s="0">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="C12" s="0">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>486</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>487</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>500</v>
+      </c>
+      <c r="I12" s="0">
+        <v>100</v>
+      </c>
+      <c r="J12" s="0">
+        <v>5</v>
+      </c>
+      <c r="M12" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="C13" s="0">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>502</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>503</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>500</v>
+      </c>
+      <c r="I13" s="0">
+        <v>9999</v>
+      </c>
+      <c r="J13" s="0">
+        <v>10</v>
+      </c>
+      <c r="M13" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="C14" s="0">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>489</v>
+      </c>
+      <c r="H14" s="0">
+        <v>25</v>
+      </c>
+      <c r="M14" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>498</v>
+      </c>
+      <c r="C15" s="0">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>479</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>472</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>499</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>500</v>
+      </c>
+      <c r="H15" s="0">
+        <v>20</v>
+      </c>
+      <c r="I15" s="0">
+        <v>30</v>
+      </c>
+      <c r="J15" s="0">
+        <v>2</v>
+      </c>
+      <c r="M15" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>471</v>
+      </c>
+      <c r="C16" s="0">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>496</v>
+      </c>
+      <c r="K16" s="0">
+        <v>10</v>
+      </c>
+      <c r="L16" s="0">
+        <v>1</v>
+      </c>
+      <c r="M16" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>498</v>
+      </c>
+      <c r="C17" s="0">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>488</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>505</v>
+      </c>
+      <c r="H17" s="0">
+        <v>30</v>
+      </c>
+      <c r="M17" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>498</v>
+      </c>
+      <c r="C18" s="0">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>496</v>
+      </c>
+      <c r="K18" s="0">
+        <v>20</v>
+      </c>
+      <c r="L18" s="0">
+        <v>9</v>
+      </c>
+      <c r="M18" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s" s="0">
+        <v>501</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="C19" s="0">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>488</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>506</v>
+      </c>
+      <c r="K19" s="0">
+        <v>10</v>
+      </c>
+      <c r="L19" s="0">
+        <v>4</v>
+      </c>
+      <c r="M19" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>